<commit_message>
Updated 2021 results file
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1228" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68B512CA-4666-4355-8BFC-379B087526D9}"/>
+  <xr:revisionPtr revIDLastSave="1292" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1214C603-1E3B-48DE-86B6-913D8FD7706F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="297">
   <si>
     <t>Type</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Giacomo Nizzolo</t>
   </si>
   <si>
-    <t>Cess Bol</t>
-  </si>
-  <si>
     <t>Elia Viviani</t>
   </si>
   <si>
@@ -763,9 +760,6 @@
     <t>Baptiste Planckaert</t>
   </si>
   <si>
-    <t>Ramus Tiller</t>
-  </si>
-  <si>
     <t>Connor Swift</t>
   </si>
   <si>
@@ -908,6 +902,30 @@
   </si>
   <si>
     <t>5h10'</t>
+  </si>
+  <si>
+    <t>Rasmus Tiller</t>
+  </si>
+  <si>
+    <t>Cees Bol</t>
+  </si>
+  <si>
+    <t>Tokyo Road Race</t>
+  </si>
+  <si>
+    <t>Orluis Aular</t>
+  </si>
+  <si>
+    <t>Elisa Longo Borghini</t>
+  </si>
+  <si>
+    <t>Coryn Rivera</t>
+  </si>
+  <si>
+    <t>Carol-Ann Canuel</t>
+  </si>
+  <si>
+    <t>Anna Kiesenhofer</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1083,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1160,12 +1178,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1173,6 +1185,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1498,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,19 +1554,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C2" s="14">
         <v>9</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>41</v>
@@ -1561,66 +1576,66 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C3" s="14">
         <v>9</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C4" s="14">
         <v>9</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C5" s="14">
         <v>9</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="4"/>
@@ -1696,7 +1711,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="14">
         <v>9</v>
@@ -1708,7 +1723,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="4"/>
@@ -1718,7 +1733,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="14">
         <v>9</v>
@@ -1730,7 +1745,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="4"/>
@@ -1740,7 +1755,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C11" s="14">
         <v>9</v>
@@ -1752,7 +1767,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="4"/>
@@ -1762,7 +1777,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C12" s="14">
         <v>9</v>
@@ -1774,7 +1789,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="4"/>
@@ -1784,7 +1799,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C13" s="14">
         <v>9</v>
@@ -1803,10 +1818,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="14">
         <v>6</v>
@@ -1818,17 +1833,17 @@
         <v>42</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C15" s="14">
         <v>6</v>
@@ -1840,17 +1855,17 @@
         <v>40</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="14">
         <v>6</v>
@@ -1862,17 +1877,17 @@
         <v>38</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C17" s="14">
         <v>6</v>
@@ -1884,17 +1899,17 @@
         <v>39</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" s="14">
         <v>6</v>
@@ -1906,17 +1921,17 @@
         <v>41</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C19" s="14">
         <v>6</v>
@@ -1928,17 +1943,17 @@
         <v>38</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C20" s="14">
         <v>6</v>
@@ -1950,31 +1965,31 @@
         <v>44</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="A21" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="14">
         <v>6</v>
       </c>
-      <c r="D21" s="1">
-        <v>50</v>
-      </c>
-      <c r="E21" s="1">
-        <v>50</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="1"/>
+      <c r="D21" s="14">
+        <v>30</v>
+      </c>
+      <c r="E21" s="14">
+        <v>30</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" s="14"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1982,19 +1997,19 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1">
         <v>6</v>
       </c>
       <c r="D22" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="2"/>
@@ -2004,19 +2019,19 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E23" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="2"/>
@@ -2026,131 +2041,131 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E24" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1">
+        <v>55</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C26" s="7">
         <v>6</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D26" s="7">
         <v>53</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E26" s="7">
         <v>53</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C27" s="9">
         <v>6</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D27" s="9">
         <v>45</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E27" s="9">
         <v>45</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="G27" s="9"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B28" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="11">
+        <v>6</v>
+      </c>
+      <c r="D28" s="11">
+        <v>44</v>
+      </c>
+      <c r="E28" s="11">
+        <v>44</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C27" s="11">
+      <c r="G28" s="11"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="12">
         <v>6</v>
       </c>
-      <c r="D27" s="11">
-        <v>44</v>
-      </c>
-      <c r="E27" s="11">
-        <v>44</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C28" s="12">
-        <v>6</v>
-      </c>
-      <c r="D28" s="12">
+      <c r="D29" s="12">
         <v>47</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E29" s="12">
         <v>47</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="14">
-        <v>6</v>
-      </c>
-      <c r="D29" s="14">
-        <v>52</v>
-      </c>
-      <c r="E29" s="14">
-        <v>52</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2158,19 +2173,19 @@
         <v>7</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="C30" s="14">
         <v>6</v>
       </c>
       <c r="D30" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E30" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="2"/>
@@ -2180,19 +2195,19 @@
         <v>7</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="C31" s="14">
         <v>6</v>
       </c>
       <c r="D31" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E31" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="2"/>
@@ -2202,19 +2217,19 @@
         <v>7</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C32" s="14">
         <v>6</v>
       </c>
       <c r="D32" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E32" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="2"/>
@@ -2224,7 +2239,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C33" s="14">
         <v>6</v>
@@ -2236,7 +2251,7 @@
         <v>55</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="2"/>
@@ -2246,19 +2261,19 @@
         <v>7</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C34" s="14">
         <v>6</v>
       </c>
       <c r="D34" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E34" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="2"/>
@@ -2268,65 +2283,65 @@
         <v>7</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="C35" s="14">
         <v>6</v>
       </c>
       <c r="D35" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E35" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>133</v>
+        <v>214</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="1">
-        <v>12</v>
-      </c>
-      <c r="D36" s="1">
-        <v>55</v>
-      </c>
-      <c r="E36" s="1">
-        <v>25</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" s="1"/>
+      <c r="A36" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C36" s="14">
+        <v>6</v>
+      </c>
+      <c r="D36" s="14">
+        <v>42</v>
+      </c>
+      <c r="E36" s="14">
+        <v>42</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G36" s="14"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="1">
-        <v>12</v>
-      </c>
-      <c r="D37" s="1">
-        <v>53</v>
-      </c>
-      <c r="E37" s="1">
-        <v>25</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G37" s="1"/>
+      <c r="A37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C37" s="14">
+        <v>6</v>
+      </c>
+      <c r="D37" s="14">
+        <v>40</v>
+      </c>
+      <c r="E37" s="14">
+        <v>40</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" s="14"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2334,19 +2349,19 @@
         <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1">
         <v>12</v>
       </c>
       <c r="D38" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E38" s="1">
         <v>25</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="2"/>
@@ -2356,19 +2371,19 @@
         <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1">
         <v>12</v>
       </c>
       <c r="D39" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E39" s="1">
         <v>25</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="2"/>
@@ -2378,13 +2393,13 @@
         <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1">
         <v>12</v>
       </c>
       <c r="D40" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E40" s="1">
         <v>25</v>
@@ -2400,19 +2415,19 @@
         <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C41" s="1">
         <v>12</v>
       </c>
       <c r="D41" s="1">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E41" s="1">
         <v>25</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
@@ -2422,19 +2437,19 @@
         <v>60</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C42" s="1">
         <v>12</v>
       </c>
       <c r="D42" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E42" s="1">
         <v>25</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="2"/>
@@ -2444,19 +2459,19 @@
         <v>60</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="C43" s="1">
         <v>12</v>
       </c>
       <c r="D43" s="1">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E43" s="1">
         <v>25</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
@@ -2466,19 +2481,19 @@
         <v>60</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="C44" s="1">
         <v>12</v>
       </c>
       <c r="D44" s="1">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E44" s="1">
         <v>25</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="2"/>
@@ -2488,19 +2503,19 @@
         <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
       <c r="C45" s="1">
         <v>12</v>
       </c>
       <c r="D45" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E45" s="1">
         <v>25</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="2"/>
@@ -2510,62 +2525,86 @@
         <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C46" s="1">
         <v>12</v>
       </c>
       <c r="D46" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E46" s="1">
         <v>25</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>219</v>
+        <v>12</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C47" s="1">
         <v>12</v>
       </c>
       <c r="D47" s="1">
+        <v>55</v>
+      </c>
+      <c r="E47" s="1">
+        <v>25</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" s="1">
+        <v>12</v>
+      </c>
+      <c r="D48" s="1">
+        <v>53</v>
+      </c>
+      <c r="E48" s="1">
+        <v>25</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C49" s="1">
+        <v>12</v>
+      </c>
+      <c r="D49" s="1">
         <v>293</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E49" s="1">
         <v>137</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="30"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="H49" s="30"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
@@ -2607,6 +2646,26 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2614,10 +2673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2627,7 +2686,7 @@
     <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="10" width="21" customWidth="1"/>
     <col min="11" max="11" width="21.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.140625" customWidth="1"/>
@@ -2645,34 +2704,34 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="K1" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J1" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>148</v>
-      </c>
       <c r="N1" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -2719,10 +2778,10 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>238</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>239</v>
       </c>
       <c r="C4" s="14">
         <v>12554</v>
@@ -2734,28 +2793,28 @@
         <v>19</v>
       </c>
       <c r="F4" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="K4" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="L4" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="M4" s="22" t="s">
         <v>252</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>254</v>
       </c>
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
@@ -2767,10 +2826,10 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C5" s="14">
         <v>13263</v>
@@ -2782,28 +2841,28 @@
         <v>51</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>52</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
@@ -2945,31 +3004,31 @@
         <v>100</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="H9" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="I9" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="K9" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="M9" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>122</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -2984,7 +3043,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="14">
         <v>5196</v>
@@ -2999,25 +3058,25 @@
         <v>51</v>
       </c>
       <c r="G10" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="J10" s="22" t="s">
         <v>170</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>171</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>29</v>
       </c>
       <c r="L10" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="M10" s="24" t="s">
         <v>172</v>
-      </c>
-      <c r="M10" s="24" t="s">
-        <v>173</v>
       </c>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
@@ -3032,7 +3091,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C11" s="14">
         <v>4393</v>
@@ -3041,31 +3100,31 @@
         <v>100</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="G11" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>69</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>62</v>
       </c>
       <c r="L11" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="M11" s="20" t="s">
         <v>236</v>
-      </c>
-      <c r="M11" s="20" t="s">
-        <v>237</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
@@ -3080,7 +3139,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C12" s="14">
         <v>5565</v>
@@ -3089,28 +3148,28 @@
         <v>100</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="G12" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I12" s="16" t="s">
         <v>264</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>266</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>69</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="L12" s="33" t="s">
-        <v>268</v>
+        <v>265</v>
+      </c>
+      <c r="L12" s="31" t="s">
+        <v>266</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>83</v>
@@ -3128,7 +3187,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C13" s="14">
         <v>4813</v>
@@ -3137,31 +3196,31 @@
         <v>100</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G13" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="H13" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="I13" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="K13" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M13" s="32" t="s">
         <v>273</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>274</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="M13" s="34" t="s">
-        <v>275</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
@@ -3176,7 +3235,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C14" s="14">
         <v>6355</v>
@@ -3185,31 +3244,31 @@
         <v>100</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="H14" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>137</v>
-      </c>
       <c r="I14" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="J14" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="K14" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="J14" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="M14" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="L14" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>285</v>
       </c>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
@@ -3243,10 +3302,10 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="14">
         <v>845</v>
@@ -3255,22 +3314,22 @@
         <v>100</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="G16" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="H16" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="I16" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="J16" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
@@ -3285,10 +3344,10 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" s="14">
         <v>910</v>
@@ -3297,22 +3356,22 @@
         <v>82</v>
       </c>
       <c r="E17" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="I17" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="J17" s="19" t="s">
         <v>165</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>166</v>
       </c>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -3327,10 +3386,10 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="14">
         <v>1150</v>
@@ -3339,22 +3398,22 @@
         <v>68</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G18" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>178</v>
       </c>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
@@ -3369,10 +3428,10 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C19" s="14">
         <v>860</v>
@@ -3381,22 +3440,22 @@
         <v>100</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="G19" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="G19" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="H19" s="16" t="s">
+      <c r="I19" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="J19" s="15" t="s">
         <v>194</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>195</v>
       </c>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
@@ -3411,10 +3470,10 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C20" s="14">
         <v>866</v>
@@ -3423,22 +3482,22 @@
         <v>100</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F20" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="F20" s="22" t="s">
-        <v>206</v>
-      </c>
       <c r="G20" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="I20" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>176</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>177</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
@@ -3453,10 +3512,10 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C21" s="14">
         <v>1016</v>
@@ -3465,22 +3524,22 @@
         <v>98</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="I21" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="J21" s="29" t="s">
         <v>213</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>214</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
@@ -3495,10 +3554,10 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C22" s="14">
         <v>933</v>
@@ -3507,22 +3566,22 @@
         <v>94</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="J22" s="36" t="s">
-        <v>139</v>
+        <v>213</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>138</v>
       </c>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -3535,69 +3594,67 @@
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
     </row>
-    <row r="23" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="1">
-        <v>727</v>
-      </c>
-      <c r="D24" s="1">
-        <v>100</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="18" t="s">
-        <v>22</v>
-      </c>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C23" s="14">
+        <v>677</v>
+      </c>
+      <c r="D23" s="14">
+        <v>98</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+    </row>
+    <row r="24" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="M24" s="37"/>
-      <c r="N24" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -3608,38 +3665,42 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1">
-        <v>505</v>
+        <v>727</v>
       </c>
       <c r="D25" s="1">
-        <v>84</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>26</v>
+        <v>100</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+      <c r="L25" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="36"/>
+      <c r="N25" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -3650,31 +3711,31 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" s="1">
-        <v>535</v>
+        <v>505</v>
       </c>
       <c r="D26" s="1">
-        <v>50</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>36</v>
+        <v>84</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -3692,31 +3753,31 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1">
-        <v>700</v>
+        <v>535</v>
       </c>
       <c r="D27" s="1">
-        <v>100</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -3730,245 +3791,245 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1">
+        <v>700</v>
+      </c>
+      <c r="D28" s="1">
+        <v>100</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C29" s="7">
         <v>669</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D29" s="7">
         <v>94</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F29" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H29" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I28" s="19" t="s">
+      <c r="I29" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="J29" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C30" s="9">
         <v>791</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D30" s="9">
         <v>98</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E30" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G30" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H30" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I29" s="19" t="s">
+      <c r="I30" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J30" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="11">
+      <c r="B31" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="11">
         <v>853</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D31" s="11">
         <v>100</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F31" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G31" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H31" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I31" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="I30" s="19" t="s">
+      <c r="J31" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="J30" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="K30" s="8"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="K31" s="8"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B32" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="13">
+        <v>740</v>
+      </c>
+      <c r="D32" s="13">
+        <v>90</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="13">
-        <v>740</v>
-      </c>
-      <c r="D31" s="13">
-        <v>90</v>
-      </c>
-      <c r="E31" s="15" t="s">
+      <c r="F32" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="G32" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31" s="17" t="s">
+      <c r="J32" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="J31" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="14">
-        <v>848</v>
-      </c>
-      <c r="D32" s="14">
-        <v>100</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="J32" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="K32" s="8"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="C33" s="14">
-        <v>519</v>
+        <v>848</v>
       </c>
       <c r="D33" s="14">
         <v>100</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>93</v>
+        <v>17</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="J33" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="K33" s="8"/>
       <c r="L33" s="14"/>
@@ -3986,31 +4047,31 @@
         <v>7</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="C34" s="14">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="D34" s="14">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J34" s="19" t="s">
-        <v>181</v>
+        <v>77</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="K34" s="8"/>
       <c r="L34" s="14"/>
@@ -4028,31 +4089,31 @@
         <v>7</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C35" s="14">
-        <v>595</v>
+        <v>503</v>
       </c>
       <c r="D35" s="14">
         <v>98</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="22" t="s">
+      <c r="F35" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="19" t="s">
         <v>180</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>48</v>
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="14"/>
@@ -4070,31 +4131,31 @@
         <v>7</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C36" s="14">
-        <v>573</v>
+        <v>595</v>
       </c>
       <c r="D36" s="14">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>173</v>
+        <v>52</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="J36" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="K36" s="8"/>
       <c r="L36" s="14"/>
@@ -4112,44 +4173,40 @@
         <v>7</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C37" s="14">
-        <v>750</v>
+        <v>573</v>
       </c>
       <c r="D37" s="14">
         <v>100</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="I37" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="J37" s="28" t="s">
-        <v>218</v>
+        <v>18</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="K37" s="8"/>
-      <c r="L37" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="39" t="s">
-        <v>227</v>
-      </c>
-      <c r="R37" s="39"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="14"/>
     </row>
@@ -4158,168 +4215,148 @@
         <v>7</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="C38" s="14">
-        <v>534</v>
+        <v>750</v>
       </c>
       <c r="D38" s="14">
-        <v>46</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="H38" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="J38" s="19" t="s">
-        <v>246</v>
+        <v>100</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J38" s="28" t="s">
+        <v>217</v>
       </c>
       <c r="K38" s="8"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
-      <c r="P38" s="31"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="32"/>
+      <c r="L38" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="R38" s="38"/>
       <c r="S38" s="14"/>
       <c r="T38" s="14"/>
     </row>
-    <row r="39" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" s="14">
+        <v>534</v>
+      </c>
+      <c r="D39" s="14">
+        <v>46</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="1">
-        <v>2470</v>
-      </c>
-      <c r="D40" s="1">
-        <v>100</v>
+      <c r="A40" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" s="14">
+        <v>830</v>
+      </c>
+      <c r="D40" s="14">
+        <v>98</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G40" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>167</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J40" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="L40" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M40" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N40" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O40" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P40" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1891</v>
-      </c>
-      <c r="D41" s="1">
-        <v>88</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F41" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I41" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="J41" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="L41" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M41" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N41" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="O41" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="P41" s="17" t="s">
-        <v>94</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="J40" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+    </row>
+    <row r="41" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
@@ -4330,49 +4367,49 @@
         <v>60</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C42" s="1">
-        <v>2256</v>
+        <v>2470</v>
       </c>
       <c r="D42" s="1">
         <v>100</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>82</v>
+        <v>63</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="K42" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="L42" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="M42" s="19" t="s">
-        <v>98</v>
+        <v>69</v>
+      </c>
+      <c r="K42" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L42" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="N42" s="18" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="O42" s="18" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="P42" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -4384,49 +4421,49 @@
         <v>60</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C43" s="1">
-        <v>2654</v>
+        <v>1891</v>
       </c>
       <c r="D43" s="1">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>110</v>
+        <v>44</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H43" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I43" s="15" t="s">
-        <v>69</v>
+      <c r="I43" s="19" t="s">
+        <v>290</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="L43" s="19" t="s">
-        <v>112</v>
+        <v>79</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="M43" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="N43" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="O43" s="19" t="s">
-        <v>108</v>
+        <v>80</v>
+      </c>
+      <c r="N43" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O43" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="P43" s="17" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -4438,49 +4475,49 @@
         <v>60</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1">
-        <v>2035</v>
+        <v>2256</v>
       </c>
       <c r="D44" s="1">
+        <v>100</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K44" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L44" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M44" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N44" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="H44" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="I44" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J44" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L44" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M44" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="N44" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="O44" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="P44" s="17" t="s">
-        <v>129</v>
+      <c r="O44" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="P44" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -4492,49 +4529,49 @@
         <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C45" s="1">
-        <v>2692</v>
+        <v>2654</v>
       </c>
       <c r="D45" s="1">
         <v>100</v>
       </c>
-      <c r="E45" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>83</v>
+      <c r="E45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="G45" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K45" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="H45" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I45" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="J45" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="K45" s="19" t="s">
+      <c r="L45" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M45" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N45" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="L45" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="M45" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="N45" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="O45" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P45" s="18" t="s">
-        <v>99</v>
+      <c r="O45" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="P45" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -4546,49 +4583,49 @@
         <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C46" s="1">
-        <v>2216</v>
+        <v>2035</v>
       </c>
       <c r="D46" s="1">
-        <v>90</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>153</v>
+        <v>127</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J46" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="L46" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="M46" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N46" s="17" t="s">
-        <v>158</v>
+        <v>84</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L46" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M46" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N46" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="O46" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="P46" s="16" t="s">
-        <v>93</v>
+        <v>111</v>
+      </c>
+      <c r="P46" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -4600,49 +4637,49 @@
         <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="C47" s="1">
-        <v>2066</v>
+        <v>2692</v>
       </c>
       <c r="D47" s="1">
         <v>100</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="G47" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="J47" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K47" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="H47" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="I47" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="J47" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="K47" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L47" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="M47" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="N47" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="O47" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="P47" s="17" t="s">
-        <v>188</v>
+      <c r="L47" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M47" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="N47" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="O47" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P47" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
@@ -4654,49 +4691,49 @@
         <v>60</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="C48" s="1">
-        <v>2680</v>
+        <v>2216</v>
       </c>
       <c r="D48" s="1">
-        <v>100</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="I48" s="22" t="s">
-        <v>198</v>
+        <v>90</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="K48" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="L48" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="M48" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="N48" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="O48" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="P48" s="25" t="s">
-        <v>203</v>
+        <v>155</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L48" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="M48" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N48" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O48" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P48" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
@@ -4708,49 +4745,49 @@
         <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
       <c r="C49" s="1">
-        <v>1771</v>
+        <v>2066</v>
       </c>
       <c r="D49" s="1">
         <v>100</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>42</v>
+      <c r="E49" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H49" s="16" t="s">
-        <v>207</v>
+        <v>110</v>
+      </c>
+      <c r="H49" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="K49" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="L49" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="M49" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="N49" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="O49" s="26" t="s">
-        <v>211</v>
+        <v>180</v>
+      </c>
+      <c r="K49" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L49" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="M49" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="N49" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="O49" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="P49" s="17" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
@@ -4762,49 +4799,49 @@
         <v>60</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C50" s="1">
-        <v>2700</v>
+        <v>2680</v>
       </c>
       <c r="D50" s="1">
         <v>100</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>216</v>
+        <v>52</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="I50" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>168</v>
+        <v>116</v>
+      </c>
+      <c r="I50" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="L50" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="M50" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="N50" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="O50" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="P50" s="27" t="s">
-        <v>225</v>
+        <v>126</v>
+      </c>
+      <c r="L50" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="M50" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="N50" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O50" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="P50" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
@@ -4812,22 +4849,54 @@
       <c r="T50" s="1"/>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1771</v>
+      </c>
+      <c r="D51" s="1">
+        <v>100</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J51" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L51" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M51" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="N51" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="O51" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="P51" s="17" t="s">
+        <v>196</v>
+      </c>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -4835,25 +4904,53 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D52" s="1">
+        <v>100</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I52" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K52" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="L52" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M52" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="N52" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="O52" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="P52" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
@@ -4882,8 +4979,12 @@
       <c r="T53" s="1"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -4925,12 +5026,56 @@
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
     </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="L37:P37"/>
-    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="L38:P38"/>
+    <mergeCell ref="Q38:R38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Donostia results
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1292" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1214C603-1E3B-48DE-86B6-913D8FD7706F}"/>
+  <xr:revisionPtr revIDLastSave="1339" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CF8FE67-0C75-4773-A95B-F66BDC67CA6B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="308">
   <si>
     <t>Type</t>
   </si>
@@ -926,6 +926,39 @@
   </si>
   <si>
     <t>Anna Kiesenhofer</t>
+  </si>
+  <si>
+    <t>Donostia</t>
+  </si>
+  <si>
+    <t>1'47''</t>
+  </si>
+  <si>
+    <t>Mikkel Honore</t>
+  </si>
+  <si>
+    <t>Lorenzo Rota</t>
+  </si>
+  <si>
+    <t>Alessandro Covi</t>
+  </si>
+  <si>
+    <t>Neilson Powless</t>
+  </si>
+  <si>
+    <t>Simon Carr</t>
+  </si>
+  <si>
+    <t>5''</t>
+  </si>
+  <si>
+    <t>Audrey Cordon-Ragot</t>
+  </si>
+  <si>
+    <t>Evita Muzic</t>
+  </si>
+  <si>
+    <t>Sabrina Stultiens</t>
   </si>
 </sst>
 </file>
@@ -1513,10 +1546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,25 +2026,25 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="A22" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C22" s="14">
         <v>6</v>
       </c>
-      <c r="D22" s="1">
-        <v>50</v>
-      </c>
-      <c r="E22" s="1">
-        <v>50</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="D22" s="14">
+        <v>36</v>
+      </c>
+      <c r="E22" s="14">
+        <v>36</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="G22" s="14"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2019,19 +2052,19 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="2"/>
@@ -2041,19 +2074,19 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E24" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2"/>
@@ -2063,131 +2096,131 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1">
         <v>6</v>
       </c>
       <c r="D25" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E25" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
+        <v>55</v>
+      </c>
+      <c r="E26" s="1">
+        <v>55</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C27" s="7">
         <v>6</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D27" s="7">
         <v>53</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E27" s="7">
         <v>53</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C28" s="9">
         <v>6</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D28" s="9">
         <v>45</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E28" s="9">
         <v>45</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F28" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="G28" s="9"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C29" s="11">
         <v>6</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D29" s="11">
         <v>44</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E29" s="11">
         <v>44</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="G29" s="11"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B30" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C30" s="12">
         <v>6</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D30" s="12">
         <v>47</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E30" s="12">
         <v>47</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F30" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="14">
-        <v>6</v>
-      </c>
-      <c r="D30" s="14">
-        <v>52</v>
-      </c>
-      <c r="E30" s="14">
-        <v>52</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="G30" s="14"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2195,19 +2228,19 @@
         <v>7</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C31" s="14">
         <v>6</v>
       </c>
       <c r="D31" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E31" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="2"/>
@@ -2217,19 +2250,19 @@
         <v>7</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C32" s="14">
         <v>6</v>
       </c>
       <c r="D32" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E32" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="2"/>
@@ -2239,19 +2272,19 @@
         <v>7</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C33" s="14">
         <v>6</v>
       </c>
       <c r="D33" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E33" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="2"/>
@@ -2261,7 +2294,7 @@
         <v>7</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C34" s="14">
         <v>6</v>
@@ -2283,19 +2316,19 @@
         <v>7</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C35" s="14">
         <v>6</v>
       </c>
       <c r="D35" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E35" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="2"/>
@@ -2305,19 +2338,19 @@
         <v>7</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C36" s="14">
         <v>6</v>
       </c>
       <c r="D36" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E36" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>132</v>
+        <v>214</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="2"/>
@@ -2327,65 +2360,65 @@
         <v>7</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="C37" s="14">
         <v>6</v>
       </c>
       <c r="D37" s="14">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E37" s="14">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="1">
-        <v>12</v>
-      </c>
-      <c r="D38" s="1">
-        <v>55</v>
-      </c>
-      <c r="E38" s="1">
-        <v>25</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" s="1"/>
+      <c r="A38" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C38" s="14">
+        <v>6</v>
+      </c>
+      <c r="D38" s="14">
+        <v>40</v>
+      </c>
+      <c r="E38" s="14">
+        <v>40</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" s="14"/>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="1">
-        <v>12</v>
-      </c>
-      <c r="D39" s="1">
-        <v>53</v>
-      </c>
-      <c r="E39" s="1">
-        <v>25</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G39" s="1"/>
+      <c r="A39" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C39" s="14">
+        <v>6</v>
+      </c>
+      <c r="D39" s="14">
+        <v>58</v>
+      </c>
+      <c r="E39" s="14">
+        <v>58</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="G39" s="14"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2393,19 +2426,19 @@
         <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C40" s="1">
         <v>12</v>
       </c>
       <c r="D40" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E40" s="1">
         <v>25</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="2"/>
@@ -2415,19 +2448,19 @@
         <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C41" s="1">
         <v>12</v>
       </c>
       <c r="D41" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E41" s="1">
         <v>25</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="2"/>
@@ -2437,13 +2470,13 @@
         <v>60</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1">
         <v>12</v>
       </c>
       <c r="D42" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E42" s="1">
         <v>25</v>
@@ -2459,19 +2492,19 @@
         <v>60</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1">
         <v>12</v>
       </c>
       <c r="D43" s="1">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E43" s="1">
         <v>25</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
@@ -2481,19 +2514,19 @@
         <v>60</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C44" s="1">
         <v>12</v>
       </c>
       <c r="D44" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E44" s="1">
         <v>25</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="2"/>
@@ -2503,19 +2536,19 @@
         <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C45" s="1">
         <v>12</v>
       </c>
       <c r="D45" s="1">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E45" s="1">
         <v>25</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="2"/>
@@ -2525,19 +2558,19 @@
         <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C46" s="1">
         <v>12</v>
       </c>
       <c r="D46" s="1">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E46" s="1">
         <v>25</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="2"/>
@@ -2547,19 +2580,19 @@
         <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C47" s="1">
         <v>12</v>
       </c>
       <c r="D47" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E47" s="1">
         <v>25</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="2"/>
@@ -2569,62 +2602,86 @@
         <v>60</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1">
         <v>12</v>
       </c>
       <c r="D48" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E48" s="1">
         <v>25</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="C49" s="1">
         <v>12</v>
       </c>
       <c r="D49" s="1">
+        <v>55</v>
+      </c>
+      <c r="E49" s="1">
+        <v>25</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C50" s="1">
+        <v>12</v>
+      </c>
+      <c r="D50" s="1">
+        <v>53</v>
+      </c>
+      <c r="E50" s="1">
+        <v>25</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C51" s="1">
+        <v>12</v>
+      </c>
+      <c r="D51" s="1">
         <v>293</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E51" s="1">
         <v>137</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="30"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="H51" s="30"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
@@ -2666,6 +2723,26 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2673,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3638,69 +3715,65 @@
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
     </row>
-    <row r="24" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1">
-        <v>727</v>
-      </c>
-      <c r="D25" s="1">
-        <v>100</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>22</v>
-      </c>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1015</v>
+      </c>
+      <c r="D24" s="14">
+        <v>74</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="K24" s="14"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+    </row>
+    <row r="25" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="36"/>
-      <c r="N25" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -3711,38 +3784,42 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1">
-        <v>505</v>
+        <v>727</v>
       </c>
       <c r="D26" s="1">
-        <v>84</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>26</v>
+        <v>100</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="L26" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="36"/>
+      <c r="N26" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -3753,31 +3830,31 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1">
-        <v>535</v>
+        <v>505</v>
       </c>
       <c r="D27" s="1">
-        <v>50</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>36</v>
+        <v>84</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -3795,31 +3872,31 @@
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1">
-        <v>700</v>
+        <v>535</v>
       </c>
       <c r="D28" s="1">
-        <v>100</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -3833,245 +3910,245 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1">
+        <v>700</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C30" s="7">
         <v>669</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D30" s="7">
         <v>94</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F30" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H30" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I29" s="19" t="s">
+      <c r="I30" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="J29" s="16" t="s">
+      <c r="J30" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C31" s="9">
         <v>791</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D31" s="9">
         <v>98</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E31" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G31" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H31" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I30" s="19" t="s">
+      <c r="I31" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J30" s="19" t="s">
+      <c r="J31" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C32" s="11">
         <v>853</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D32" s="11">
         <v>100</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F32" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="G32" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H32" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I31" s="19" t="s">
+      <c r="I32" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J32" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="K32" s="8"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C33" s="13">
         <v>740</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D33" s="13">
         <v>90</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E33" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H33" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I33" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="J32" s="16" t="s">
+      <c r="J33" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C33" s="14">
-        <v>848</v>
-      </c>
-      <c r="D33" s="14">
-        <v>100</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="J33" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C34" s="14">
-        <v>519</v>
+        <v>848</v>
       </c>
       <c r="D34" s="14">
         <v>100</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>92</v>
+        <v>17</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="J34" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="K34" s="8"/>
       <c r="L34" s="14"/>
@@ -4089,31 +4166,31 @@
         <v>7</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C35" s="14">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="D35" s="14">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J35" s="19" t="s">
-        <v>180</v>
+        <v>77</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="14"/>
@@ -4131,31 +4208,31 @@
         <v>7</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C36" s="14">
-        <v>595</v>
+        <v>503</v>
       </c>
       <c r="D36" s="14">
         <v>98</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="22" t="s">
+      <c r="F36" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H36" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="I36" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="J36" s="20" t="s">
-        <v>48</v>
+      <c r="G36" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="K36" s="8"/>
       <c r="L36" s="14"/>
@@ -4173,31 +4250,31 @@
         <v>7</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C37" s="14">
-        <v>573</v>
+        <v>595</v>
       </c>
       <c r="D37" s="14">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H37" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="I37" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I37" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="J37" s="17" t="s">
-        <v>172</v>
+      <c r="J37" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="K37" s="8"/>
       <c r="L37" s="14"/>
@@ -4215,44 +4292,40 @@
         <v>7</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C38" s="14">
-        <v>750</v>
+        <v>573</v>
       </c>
       <c r="D38" s="14">
         <v>100</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G38" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="I38" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J38" s="28" t="s">
-        <v>217</v>
+      <c r="H38" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="K38" s="8"/>
-      <c r="L38" s="37" t="s">
-        <v>225</v>
-      </c>
-      <c r="M38" s="37"/>
-      <c r="N38" s="37"/>
-      <c r="O38" s="37"/>
-      <c r="P38" s="37"/>
-      <c r="Q38" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="R38" s="38"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
       <c r="S38" s="14"/>
       <c r="T38" s="14"/>
     </row>
@@ -4261,40 +4334,44 @@
         <v>7</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C39" s="14">
-        <v>534</v>
+        <v>750</v>
       </c>
       <c r="D39" s="14">
-        <v>46</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="J39" s="19" t="s">
-        <v>244</v>
+        <v>100</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J39" s="28" t="s">
+        <v>217</v>
       </c>
       <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
+      <c r="L39" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="R39" s="38"/>
       <c r="S39" s="14"/>
       <c r="T39" s="14"/>
     </row>
@@ -4303,31 +4380,31 @@
         <v>7</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="C40" s="14">
-        <v>830</v>
+        <v>534</v>
       </c>
       <c r="D40" s="14">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="J40" s="35" t="s">
-        <v>292</v>
+        <v>240</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>244</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -4340,131 +4417,107 @@
       <c r="S40" s="14"/>
       <c r="T40" s="14"/>
     </row>
-    <row r="41" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C41" s="14">
+        <v>830</v>
+      </c>
+      <c r="D41" s="14">
+        <v>98</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="J41" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="1">
-        <v>2470</v>
-      </c>
-      <c r="D42" s="1">
-        <v>100</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I42" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J42" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K42" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="L42" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M42" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N42" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O42" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P42" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1891</v>
-      </c>
-      <c r="D43" s="1">
-        <v>88</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="J43" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K43" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="L43" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M43" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N43" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="O43" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="P43" s="17" t="s">
-        <v>93</v>
-      </c>
+      <c r="A42" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C42" s="14">
+        <v>818</v>
+      </c>
+      <c r="D42" s="14">
+        <v>68</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+    </row>
+    <row r="43" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
@@ -4475,49 +4528,49 @@
         <v>60</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C44" s="1">
-        <v>2256</v>
+        <v>2470</v>
       </c>
       <c r="D44" s="1">
         <v>100</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>82</v>
+        <v>63</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="K44" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L44" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="M44" s="19" t="s">
-        <v>97</v>
+        <v>69</v>
+      </c>
+      <c r="K44" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L44" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M44" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="N44" s="18" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="O44" s="18" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="P44" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -4529,49 +4582,49 @@
         <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C45" s="1">
-        <v>2654</v>
+        <v>1891</v>
       </c>
       <c r="D45" s="1">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>109</v>
+        <v>44</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H45" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H45" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I45" s="15" t="s">
-        <v>69</v>
+      <c r="I45" s="19" t="s">
+        <v>290</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L45" s="19" t="s">
-        <v>111</v>
+        <v>79</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="M45" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N45" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O45" s="19" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="N45" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O45" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="P45" s="17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -4583,49 +4636,49 @@
         <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C46" s="1">
-        <v>2035</v>
+        <v>2256</v>
       </c>
       <c r="D46" s="1">
+        <v>100</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L46" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M46" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N46" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="I46" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J46" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L46" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M46" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="N46" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="O46" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>128</v>
+      <c r="O46" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="P46" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -4637,49 +4690,49 @@
         <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C47" s="1">
-        <v>2692</v>
+        <v>2654</v>
       </c>
       <c r="D47" s="1">
         <v>100</v>
       </c>
-      <c r="E47" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>83</v>
+      <c r="E47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>143</v>
+        <v>110</v>
+      </c>
+      <c r="H47" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="J47" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K47" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L47" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M47" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K47" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="L47" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M47" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="N47" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="O47" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P47" s="18" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="O47" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="P47" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
@@ -4691,49 +4744,49 @@
         <v>60</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C48" s="1">
-        <v>2216</v>
+        <v>2035</v>
       </c>
       <c r="D48" s="1">
-        <v>90</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>152</v>
+        <v>127</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="K48" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L48" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="M48" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N48" s="17" t="s">
-        <v>157</v>
+        <v>84</v>
+      </c>
+      <c r="J48" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L48" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M48" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N48" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="O48" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="P48" s="16" t="s">
-        <v>92</v>
+        <v>111</v>
+      </c>
+      <c r="P48" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
@@ -4745,49 +4798,49 @@
         <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C49" s="1">
-        <v>2066</v>
+        <v>2692</v>
       </c>
       <c r="D49" s="1">
         <v>100</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>179</v>
+        <v>83</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H49" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="I49" s="19" t="s">
-        <v>182</v>
+        <v>95</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="K49" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L49" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="M49" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="N49" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="O49" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="P49" s="17" t="s">
-        <v>187</v>
+        <v>97</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M49" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="N49" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="O49" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P49" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
@@ -4799,49 +4852,49 @@
         <v>60</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C50" s="1">
-        <v>2680</v>
+        <v>2216</v>
       </c>
       <c r="D50" s="1">
-        <v>100</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I50" s="22" t="s">
-        <v>197</v>
+        <v>90</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I50" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K50" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="L50" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="M50" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N50" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="O50" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="P50" s="25" t="s">
-        <v>202</v>
+        <v>155</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L50" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="M50" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N50" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O50" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P50" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
@@ -4853,49 +4906,49 @@
         <v>60</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C51" s="1">
-        <v>1771</v>
+        <v>2066</v>
       </c>
       <c r="D51" s="1">
         <v>100</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="22" t="s">
-        <v>42</v>
+      <c r="E51" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H51" s="16" t="s">
-        <v>206</v>
+        <v>110</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K51" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="L51" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="M51" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="N51" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O51" s="26" t="s">
-        <v>210</v>
+        <v>180</v>
+      </c>
+      <c r="K51" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L51" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="M51" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="N51" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="O51" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="P51" s="17" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
@@ -4907,49 +4960,49 @@
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C52" s="1">
-        <v>2700</v>
+        <v>2680</v>
       </c>
       <c r="D52" s="1">
         <v>100</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>215</v>
+        <v>52</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="G52" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H52" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H52" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="I52" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J52" s="6" t="s">
-        <v>167</v>
+      <c r="I52" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J52" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="K52" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="L52" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M52" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="N52" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="O52" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="P52" s="27" t="s">
-        <v>224</v>
+        <v>126</v>
+      </c>
+      <c r="L52" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="M52" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="N52" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O52" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="P52" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
@@ -4957,22 +5010,54 @@
       <c r="T52" s="1"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1771</v>
+      </c>
+      <c r="D53" s="1">
+        <v>100</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I53" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J53" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K53" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L53" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M53" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="N53" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="O53" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="P53" s="17" t="s">
+        <v>196</v>
+      </c>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
@@ -4980,25 +5065,53 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D54" s="1">
+        <v>100</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K54" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="L54" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M54" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="N54" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="O54" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="P54" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
@@ -5027,8 +5140,12 @@
       <c r="T55" s="1"/>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -5070,12 +5187,56 @@
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
     </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="L38:P38"/>
-    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="L39:P39"/>
+    <mergeCell ref="Q39:R39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Tour of Britain results
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1572" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F61512A-3D8D-40F6-A29F-56526466B7B8}"/>
+  <xr:revisionPtr revIDLastSave="1588" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02F57618-4139-4E62-855B-0A2463E750D5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="369">
   <si>
     <t>Type</t>
   </si>
@@ -985,9 +985,6 @@
     <t>Plouay</t>
   </si>
   <si>
-    <t>Madrid Challenge</t>
-  </si>
-  <si>
     <t>Benelux Tour</t>
   </si>
   <si>
@@ -1127,6 +1124,24 @@
   </si>
   <si>
     <t>Miguel Angel Lopez</t>
+  </si>
+  <si>
+    <t>Ceratizit Challenge</t>
+  </si>
+  <si>
+    <t>38''</t>
+  </si>
+  <si>
+    <t>Rory Townsend</t>
+  </si>
+  <si>
+    <t>Robin Carpenter</t>
+  </si>
+  <si>
+    <t>Jacob Scott</t>
+  </si>
+  <si>
+    <t>Matthew Gibson</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1271,12 +1286,6 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1290,7 +1299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1404,9 +1413,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1725,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,7 +1826,7 @@
         <v>314</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>304</v>
@@ -2083,7 +2089,7 @@
         <v>29</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="4"/>
@@ -2105,7 +2111,7 @@
         <v>28</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="4"/>
@@ -2127,7 +2133,7 @@
         <v>26</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="4"/>
@@ -2149,7 +2155,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="4"/>
@@ -2159,7 +2165,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C20" s="14">
         <v>9</v>
@@ -2181,7 +2187,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>316</v>
+        <v>363</v>
       </c>
       <c r="C21" s="14">
         <v>9</v>
@@ -2193,7 +2199,7 @@
         <v>26</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="4"/>
@@ -2203,7 +2209,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C22" s="14">
         <v>9</v>
@@ -2211,10 +2217,14 @@
       <c r="D22" s="14">
         <v>107</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="E22" s="14">
+        <v>29</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>364</v>
+      </c>
       <c r="G22" s="14"/>
-      <c r="H22" s="39"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
@@ -2431,7 +2441,7 @@
         <v>41</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="2"/>
@@ -3163,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3380,25 +3390,25 @@
         <v>113</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>264</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>234</v>
       </c>
       <c r="K6" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="M6" s="8" t="s">
         <v>361</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>362</v>
       </c>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
@@ -3828,31 +3838,31 @@
         <v>100</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="H16" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="K16" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="L16" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="M16" s="8" t="s">
         <v>331</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>332</v>
       </c>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
@@ -3879,28 +3889,28 @@
         <v>245</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>299</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>196</v>
       </c>
       <c r="L17" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>336</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>337</v>
       </c>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
@@ -3936,19 +3946,19 @@
         <v>137</v>
       </c>
       <c r="I18" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="K18" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="L18" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="M18" s="8" t="s">
         <v>341</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>342</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
@@ -3975,28 +3985,28 @@
         <v>190</v>
       </c>
       <c r="F19" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="K19" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>348</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
@@ -4011,7 +4021,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C20" s="14">
         <v>4931</v>
@@ -4038,13 +4048,13 @@
         <v>152</v>
       </c>
       <c r="K20" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="M20" s="8" t="s">
         <v>350</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>351</v>
       </c>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
@@ -4059,7 +4069,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>316</v>
+        <v>363</v>
       </c>
       <c r="C21" s="14">
         <v>3947</v>
@@ -4071,28 +4081,28 @@
         <v>133</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>205</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="K21" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="M21" s="8" t="s">
         <v>356</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>357</v>
       </c>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
@@ -4107,19 +4117,41 @@
         <v>37</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+        <v>317</v>
+      </c>
+      <c r="C22" s="14">
+        <v>5841</v>
+      </c>
+      <c r="D22" s="14">
+        <v>100</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>368</v>
+      </c>
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
@@ -4547,10 +4579,10 @@
         <v>293</v>
       </c>
       <c r="F33" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
Updated with GP de Wallonie results
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1588" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02F57618-4139-4E62-855B-0A2463E750D5}"/>
+  <xr:revisionPtr revIDLastSave="1606" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{365FFC93-A10E-4E84-A4EC-8E859418FE85}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="372">
   <si>
     <t>Type</t>
   </si>
@@ -1142,6 +1142,15 @@
   </si>
   <si>
     <t>Matthew Gibson</t>
+  </si>
+  <si>
+    <t>Wallonie</t>
+  </si>
+  <si>
+    <t>40''</t>
+  </si>
+  <si>
+    <t>Dorian Godon</t>
   </si>
 </sst>
 </file>
@@ -1729,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2843,25 +2852,25 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="1">
-        <v>12</v>
-      </c>
-      <c r="D51" s="1">
-        <v>55</v>
-      </c>
-      <c r="E51" s="1">
-        <v>25</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G51" s="1"/>
+      <c r="A51" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C51" s="14">
+        <v>6</v>
+      </c>
+      <c r="D51" s="14">
+        <v>50</v>
+      </c>
+      <c r="E51" s="14">
+        <v>50</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G51" s="14"/>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2869,19 +2878,19 @@
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C52" s="1">
         <v>12</v>
       </c>
       <c r="D52" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E52" s="1">
         <v>25</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="2"/>
@@ -2891,19 +2900,19 @@
         <v>60</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="1">
         <v>12</v>
       </c>
       <c r="D53" s="1">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E53" s="1">
         <v>25</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="2"/>
@@ -2913,19 +2922,19 @@
         <v>60</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C54" s="1">
         <v>12</v>
       </c>
       <c r="D54" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E54" s="1">
         <v>25</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="2"/>
@@ -2935,19 +2944,19 @@
         <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C55" s="1">
         <v>12</v>
       </c>
       <c r="D55" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E55" s="1">
         <v>25</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="2"/>
@@ -2957,19 +2966,19 @@
         <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C56" s="1">
         <v>12</v>
       </c>
       <c r="D56" s="1">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E56" s="1">
         <v>25</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="2"/>
@@ -2979,19 +2988,19 @@
         <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C57" s="1">
         <v>12</v>
       </c>
       <c r="D57" s="1">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E57" s="1">
         <v>25</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="2"/>
@@ -3001,19 +3010,19 @@
         <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C58" s="1">
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E58" s="1">
         <v>25</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="2"/>
@@ -3023,19 +3032,19 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C59" s="1">
         <v>12</v>
       </c>
       <c r="D59" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E59" s="1">
         <v>25</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="2"/>
@@ -3045,7 +3054,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C60" s="1">
         <v>12</v>
@@ -3057,7 +3066,7 @@
         <v>25</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="2"/>
@@ -3067,52 +3076,64 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C61" s="1">
         <v>12</v>
       </c>
       <c r="D61" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E61" s="1">
         <v>25</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>218</v>
+        <v>89</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="C62" s="1">
         <v>12</v>
       </c>
       <c r="D62" s="1">
+        <v>53</v>
+      </c>
+      <c r="E62" s="1">
+        <v>25</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="1">
+        <v>12</v>
+      </c>
+      <c r="D63" s="1">
         <v>293</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E63" s="1">
         <v>137</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="30"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
+      <c r="H63" s="30"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -3164,6 +3185,16 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3171,10 +3202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
-  <dimension ref="A1:T69"/>
+  <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5390,77 +5421,65 @@
       <c r="S52" s="14"/>
       <c r="T52" s="14"/>
     </row>
-    <row r="53" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="1">
-        <v>2470</v>
-      </c>
-      <c r="D54" s="1">
-        <v>100</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G54" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I54" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J54" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K54" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="L54" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M54" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N54" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O54" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P54" s="18" t="s">
-        <v>67</v>
-      </c>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C53" s="14">
+        <v>455</v>
+      </c>
+      <c r="D53" s="14">
+        <v>68</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+    </row>
+    <row r="54" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
@@ -5471,49 +5490,49 @@
         <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C55" s="1">
-        <v>1891</v>
+        <v>2470</v>
       </c>
       <c r="D55" s="1">
-        <v>88</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F55" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>90</v>
+        <v>100</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>290</v>
+        <v>65</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K55" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="L55" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M55" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N55" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="O55" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="P55" s="17" t="s">
-        <v>93</v>
+        <v>69</v>
+      </c>
+      <c r="K55" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L55" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M55" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="N55" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="O55" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="P55" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
@@ -5525,49 +5544,49 @@
         <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" s="1">
-        <v>2256</v>
+        <v>1891</v>
       </c>
       <c r="D56" s="1">
-        <v>100</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>95</v>
+        <v>290</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K56" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L56" s="19" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="M56" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N56" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="O56" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="P56" s="18" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="N56" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O56" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="P56" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
@@ -5579,49 +5598,49 @@
         <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C57" s="1">
-        <v>2654</v>
+        <v>2256</v>
       </c>
       <c r="D57" s="1">
         <v>100</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H57" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I57" s="15" t="s">
-        <v>69</v>
+      <c r="E57" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="K57" s="19" t="s">
         <v>96</v>
       </c>
       <c r="L57" s="19" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="M57" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="N57" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O57" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="P57" s="17" t="s">
-        <v>108</v>
+      <c r="N57" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="O57" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="P57" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
@@ -5633,49 +5652,49 @@
         <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C58" s="1">
-        <v>2035</v>
+        <v>2654</v>
       </c>
       <c r="D58" s="1">
-        <v>98</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="H58" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="I58" s="19" t="s">
-        <v>84</v>
+        <v>100</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H58" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I58" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K58" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K58" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="L58" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M58" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="N58" s="16" t="s">
-        <v>126</v>
+      <c r="L58" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M58" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N58" s="17" t="s">
+        <v>112</v>
       </c>
       <c r="O58" s="19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="P58" s="17" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -5687,49 +5706,49 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C59" s="1">
-        <v>2692</v>
+        <v>2035</v>
       </c>
       <c r="D59" s="1">
-        <v>100</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G59" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H59" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="H59" s="15" t="s">
+      <c r="I59" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="J59" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="I59" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="J59" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="K59" s="19" t="s">
+      <c r="K59" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L59" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N59" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="O59" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="L59" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M59" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="N59" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="O59" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P59" s="18" t="s">
-        <v>98</v>
+      <c r="P59" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
@@ -5741,49 +5760,49 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C60" s="1">
-        <v>2216</v>
+        <v>2692</v>
       </c>
       <c r="D60" s="1">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G60" s="19" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="I60" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J60" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="K60" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L60" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="M60" s="19" t="s">
-        <v>34</v>
+        <v>64</v>
+      </c>
+      <c r="I60" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="J60" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K60" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L60" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="N60" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="O60" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="P60" s="16" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="O60" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P60" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -5795,49 +5814,49 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C61" s="1">
-        <v>2066</v>
+        <v>2216</v>
       </c>
       <c r="D61" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H61" s="19" t="s">
-        <v>181</v>
+        <v>77</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="J61" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="K61" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L61" s="16" t="s">
-        <v>183</v>
+        <v>90</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="M61" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="N61" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="O61" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="P61" s="17" t="s">
-        <v>187</v>
+        <v>34</v>
+      </c>
+      <c r="N61" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O61" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P61" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5849,49 +5868,49 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C62" s="1">
-        <v>2680</v>
+        <v>2066</v>
       </c>
       <c r="D62" s="1">
         <v>100</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F62" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G62" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H62" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I62" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="J62" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K62" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="L62" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="M62" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N62" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="O62" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="P62" s="25" t="s">
-        <v>202</v>
+      <c r="F62" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="I62" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="J62" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K62" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L62" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="M62" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="N62" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="O62" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="P62" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -5903,49 +5922,49 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C63" s="1">
-        <v>1771</v>
+        <v>2680</v>
       </c>
       <c r="D63" s="1">
         <v>100</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G63" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H63" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H63" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="I63" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="J63" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K63" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="L63" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="M63" s="26" t="s">
+      <c r="I63" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J63" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="K63" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L63" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="N63" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O63" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="P63" s="17" t="s">
-        <v>196</v>
+      <c r="M63" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="N63" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O63" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="P63" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
@@ -5957,49 +5976,49 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C64" s="1">
-        <v>2700</v>
+        <v>1771</v>
       </c>
       <c r="D64" s="1">
         <v>100</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G64" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G64" s="6" t="s">
         <v>116</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="I64" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J64" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I64" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="K64" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="L64" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M64" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="N64" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="O64" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="P64" s="27" t="s">
-        <v>224</v>
+      <c r="J64" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K64" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L64" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M64" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="N64" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="O64" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="P64" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
@@ -6007,34 +6026,62 @@
       <c r="T64" s="1"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D65" s="1">
+        <v>100</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H65" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I65" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K65" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="L65" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M65" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="N65" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="O65" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="P65" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>230</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -6055,8 +6102,12 @@
       <c r="T66" s="1"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
+      <c r="A67" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -6120,6 +6171,28 @@
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
     </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L35:M35"/>

</xml_diff>

<commit_message>
Updated with Eschborn-Frankfurt results
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1606" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{365FFC93-A10E-4E84-A4EC-8E859418FE85}"/>
+  <xr:revisionPtr revIDLastSave="1644" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{329E670D-5FEC-429A-9172-FC919C1F713D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="381">
   <si>
     <t>Type</t>
   </si>
@@ -1151,6 +1151,33 @@
   </si>
   <si>
     <t>Dorian Godon</t>
+  </si>
+  <si>
+    <t>Primus Classic</t>
+  </si>
+  <si>
+    <t>Eschborn Frankfurt</t>
+  </si>
+  <si>
+    <t>Simon Clarke</t>
+  </si>
+  <si>
+    <t>Mikkel  Honore</t>
+  </si>
+  <si>
+    <t>1'44''</t>
+  </si>
+  <si>
+    <t>John Degenkolb</t>
+  </si>
+  <si>
+    <t>Andrea Pasqualon</t>
+  </si>
+  <si>
+    <t>Mike Teunissen</t>
+  </si>
+  <si>
+    <t>Fred Wright</t>
   </si>
 </sst>
 </file>
@@ -1738,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,47 +2901,47 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="1">
-        <v>12</v>
-      </c>
-      <c r="D52" s="1">
-        <v>55</v>
-      </c>
-      <c r="E52" s="1">
-        <v>25</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="1"/>
+      <c r="A52" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="C52" s="14">
+        <v>6</v>
+      </c>
+      <c r="D52" s="14">
+        <v>44</v>
+      </c>
+      <c r="E52" s="14">
+        <v>44</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G52" s="14"/>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="1">
-        <v>12</v>
-      </c>
-      <c r="D53" s="1">
-        <v>53</v>
-      </c>
-      <c r="E53" s="1">
-        <v>25</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G53" s="1"/>
+      <c r="A53" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C53" s="14">
+        <v>6</v>
+      </c>
+      <c r="D53" s="14">
+        <v>58</v>
+      </c>
+      <c r="E53" s="14">
+        <v>58</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="G53" s="14"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2922,19 +2949,19 @@
         <v>60</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C54" s="1">
         <v>12</v>
       </c>
       <c r="D54" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E54" s="1">
         <v>25</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="2"/>
@@ -2944,19 +2971,19 @@
         <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C55" s="1">
         <v>12</v>
       </c>
       <c r="D55" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E55" s="1">
         <v>25</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="2"/>
@@ -2966,13 +2993,13 @@
         <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C56" s="1">
         <v>12</v>
       </c>
       <c r="D56" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E56" s="1">
         <v>25</v>
@@ -2988,19 +3015,19 @@
         <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C57" s="1">
         <v>12</v>
       </c>
       <c r="D57" s="1">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E57" s="1">
         <v>25</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="2"/>
@@ -3010,19 +3037,19 @@
         <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C58" s="1">
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E58" s="1">
         <v>25</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="2"/>
@@ -3032,19 +3059,19 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C59" s="1">
         <v>12</v>
       </c>
       <c r="D59" s="1">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E59" s="1">
         <v>25</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="2"/>
@@ -3054,19 +3081,19 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C60" s="1">
         <v>12</v>
       </c>
       <c r="D60" s="1">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E60" s="1">
         <v>25</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="2"/>
@@ -3076,19 +3103,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C61" s="1">
         <v>12</v>
       </c>
       <c r="D61" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E61" s="1">
         <v>25</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="2"/>
@@ -3098,62 +3125,86 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C62" s="1">
         <v>12</v>
       </c>
       <c r="D62" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E62" s="1">
         <v>25</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="C63" s="1">
         <v>12</v>
       </c>
       <c r="D63" s="1">
+        <v>55</v>
+      </c>
+      <c r="E63" s="1">
+        <v>25</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C64" s="1">
+        <v>12</v>
+      </c>
+      <c r="D64" s="1">
+        <v>53</v>
+      </c>
+      <c r="E64" s="1">
+        <v>25</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C65" s="1">
+        <v>12</v>
+      </c>
+      <c r="D65" s="1">
         <v>293</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E65" s="1">
         <v>137</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="30"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+      <c r="H65" s="30"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
@@ -3195,6 +3246,26 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3202,10 +3273,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
-  <dimension ref="A1:T70"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5463,131 +5534,107 @@
       <c r="S53" s="14"/>
       <c r="T53" s="14"/>
     </row>
-    <row r="54" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1"/>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="C54" s="14">
+        <v>585</v>
+      </c>
+      <c r="D54" s="14">
+        <v>100</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="1">
-        <v>2470</v>
-      </c>
-      <c r="D55" s="1">
+      <c r="A55" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C55" s="14">
+        <v>661</v>
+      </c>
+      <c r="D55" s="14">
         <v>100</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G55" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J55" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K55" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="L55" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M55" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N55" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O55" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P55" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1891</v>
-      </c>
-      <c r="D56" s="1">
-        <v>88</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F56" s="22" t="s">
+      <c r="E55" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G56" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H56" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I56" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="J56" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K56" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="L56" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M56" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N56" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="O56" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="P56" s="17" t="s">
-        <v>93</v>
-      </c>
+      <c r="F55" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+    </row>
+    <row r="56" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
@@ -5598,49 +5645,49 @@
         <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C57" s="1">
-        <v>2256</v>
+        <v>2470</v>
       </c>
       <c r="D57" s="1">
         <v>100</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>82</v>
+        <v>63</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="K57" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L57" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="M57" s="19" t="s">
-        <v>97</v>
+        <v>69</v>
+      </c>
+      <c r="K57" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L57" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M57" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="N57" s="18" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="O57" s="18" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="P57" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
@@ -5652,49 +5699,49 @@
         <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C58" s="1">
-        <v>2654</v>
+        <v>1891</v>
       </c>
       <c r="D58" s="1">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>109</v>
+        <v>44</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H58" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H58" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I58" s="15" t="s">
-        <v>69</v>
+      <c r="I58" s="19" t="s">
+        <v>290</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K58" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L58" s="19" t="s">
-        <v>111</v>
+        <v>79</v>
+      </c>
+      <c r="L58" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="M58" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N58" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O58" s="19" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="N58" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O58" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="P58" s="17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -5706,49 +5753,49 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C59" s="1">
-        <v>2035</v>
+        <v>2256</v>
       </c>
       <c r="D59" s="1">
+        <v>100</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I59" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J59" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K59" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L59" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M59" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N59" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F59" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G59" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="H59" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="I59" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J59" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L59" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M59" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="N59" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="O59" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="P59" s="17" t="s">
-        <v>128</v>
+      <c r="O59" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="P59" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
@@ -5760,49 +5807,49 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C60" s="1">
-        <v>2692</v>
+        <v>2654</v>
       </c>
       <c r="D60" s="1">
         <v>100</v>
       </c>
-      <c r="E60" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>83</v>
+      <c r="E60" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I60" s="16" t="s">
-        <v>143</v>
+        <v>110</v>
+      </c>
+      <c r="H60" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I60" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="J60" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K60" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L60" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M60" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K60" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="L60" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M60" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="N60" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="O60" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P60" s="18" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="O60" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="P60" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -5814,49 +5861,49 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C61" s="1">
-        <v>2216</v>
+        <v>2035</v>
       </c>
       <c r="D61" s="1">
-        <v>90</v>
-      </c>
-      <c r="E61" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>152</v>
+        <v>127</v>
+      </c>
+      <c r="H61" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J61" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="K61" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L61" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="M61" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N61" s="17" t="s">
-        <v>157</v>
+        <v>84</v>
+      </c>
+      <c r="J61" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L61" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N61" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="O61" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="P61" s="16" t="s">
-        <v>92</v>
+        <v>111</v>
+      </c>
+      <c r="P61" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5868,49 +5915,49 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C62" s="1">
-        <v>2066</v>
+        <v>2692</v>
       </c>
       <c r="D62" s="1">
         <v>100</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>179</v>
+        <v>83</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H62" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="I62" s="19" t="s">
-        <v>182</v>
+        <v>95</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="K62" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L62" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="M62" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="N62" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="O62" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="P62" s="17" t="s">
-        <v>187</v>
+        <v>97</v>
+      </c>
+      <c r="K62" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L62" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M62" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="N62" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="O62" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P62" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -5922,49 +5969,49 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C63" s="1">
-        <v>2680</v>
+        <v>2216</v>
       </c>
       <c r="D63" s="1">
-        <v>100</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G63" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H63" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I63" s="22" t="s">
-        <v>197</v>
+        <v>90</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I63" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="J63" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K63" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="L63" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="M63" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N63" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="O63" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="P63" s="25" t="s">
-        <v>202</v>
+        <v>155</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L63" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="M63" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N63" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O63" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P63" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
@@ -5976,49 +6023,49 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C64" s="1">
-        <v>1771</v>
+        <v>2066</v>
       </c>
       <c r="D64" s="1">
         <v>100</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="22" t="s">
-        <v>42</v>
+      <c r="E64" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>206</v>
+        <v>110</v>
+      </c>
+      <c r="H64" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="I64" s="19" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="J64" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K64" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="L64" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="M64" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="N64" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O64" s="26" t="s">
-        <v>210</v>
+        <v>180</v>
+      </c>
+      <c r="K64" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L64" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="M64" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="N64" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="O64" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="P64" s="17" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
@@ -6030,49 +6077,49 @@
         <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C65" s="1">
-        <v>2700</v>
+        <v>2680</v>
       </c>
       <c r="D65" s="1">
         <v>100</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F65" s="17" t="s">
-        <v>215</v>
+        <v>52</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="G65" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H65" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H65" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="I65" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>167</v>
+      <c r="I65" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J65" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="K65" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="L65" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M65" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="N65" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="O65" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="P65" s="27" t="s">
-        <v>224</v>
+        <v>126</v>
+      </c>
+      <c r="L65" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="M65" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="N65" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O65" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="P65" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
@@ -6080,22 +6127,54 @@
       <c r="T65" s="1"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1771</v>
+      </c>
+      <c r="D66" s="1">
+        <v>100</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H66" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J66" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K66" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L66" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M66" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="N66" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="O66" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="P66" s="17" t="s">
+        <v>196</v>
+      </c>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
@@ -6103,25 +6182,53 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D67" s="1">
+        <v>100</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I67" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K67" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="L67" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M67" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="N67" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="O67" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="P67" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
@@ -6150,8 +6257,12 @@
       <c r="T68" s="1"/>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -6193,6 +6304,50 @@
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
     </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L35:M35"/>

</xml_diff>

<commit_message>
Updated with Worlds M and F results
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1644" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{329E670D-5FEC-429A-9172-FC919C1F713D}"/>
+  <xr:revisionPtr revIDLastSave="1679" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C24772-63F4-423A-B996-4EA2EF480E6E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="383">
   <si>
     <t>Type</t>
   </si>
@@ -1178,6 +1178,12 @@
   </si>
   <si>
     <t>Fred Wright</t>
+  </si>
+  <si>
+    <t>Worlds Road Race</t>
+  </si>
+  <si>
+    <t>Michael Valgren</t>
   </si>
 </sst>
 </file>
@@ -1765,10 +1771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,25 +2489,25 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="A33" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C33" s="14">
         <v>6</v>
       </c>
-      <c r="D33" s="1">
-        <v>50</v>
-      </c>
-      <c r="E33" s="1">
-        <v>50</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="1"/>
+      <c r="D33" s="14">
+        <v>37</v>
+      </c>
+      <c r="E33" s="14">
+        <v>37</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G33" s="14"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2509,19 +2515,19 @@
         <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1">
         <v>6</v>
       </c>
       <c r="D34" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E34" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>
@@ -2531,19 +2537,19 @@
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35" s="1">
         <v>6</v>
       </c>
       <c r="D35" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
@@ -2553,131 +2559,131 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1">
         <v>6</v>
       </c>
       <c r="D36" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E36" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="1">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1">
+        <v>55</v>
+      </c>
+      <c r="E37" s="1">
+        <v>55</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C38" s="7">
         <v>6</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D38" s="7">
         <v>53</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E38" s="7">
         <v>53</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="G38" s="7"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C39" s="9">
         <v>6</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D39" s="9">
         <v>45</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E39" s="9">
         <v>45</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="G39" s="9"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B40" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C40" s="11">
         <v>6</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D40" s="11">
         <v>44</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E40" s="11">
         <v>44</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F40" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="G40" s="11"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B41" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C41" s="12">
         <v>6</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D41" s="12">
         <v>47</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E41" s="12">
         <v>47</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F41" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="14">
-        <v>6</v>
-      </c>
-      <c r="D41" s="14">
-        <v>52</v>
-      </c>
-      <c r="E41" s="14">
-        <v>52</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="G41" s="14"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2685,19 +2691,19 @@
         <v>7</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C42" s="14">
         <v>6</v>
       </c>
       <c r="D42" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E42" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="G42" s="14"/>
       <c r="H42" s="2"/>
@@ -2707,19 +2713,19 @@
         <v>7</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C43" s="14">
         <v>6</v>
       </c>
       <c r="D43" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E43" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="G43" s="14"/>
       <c r="H43" s="2"/>
@@ -2729,19 +2735,19 @@
         <v>7</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C44" s="14">
         <v>6</v>
       </c>
       <c r="D44" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E44" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="2"/>
@@ -2751,7 +2757,7 @@
         <v>7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C45" s="14">
         <v>6</v>
@@ -2773,19 +2779,19 @@
         <v>7</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C46" s="14">
         <v>6</v>
       </c>
       <c r="D46" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E46" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="2"/>
@@ -2795,19 +2801,19 @@
         <v>7</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C47" s="14">
         <v>6</v>
       </c>
       <c r="D47" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E47" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>132</v>
+        <v>214</v>
       </c>
       <c r="G47" s="14"/>
       <c r="H47" s="2"/>
@@ -2817,19 +2823,19 @@
         <v>7</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="C48" s="14">
         <v>6</v>
       </c>
       <c r="D48" s="14">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E48" s="14">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="2"/>
@@ -2839,19 +2845,19 @@
         <v>7</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C49" s="14">
         <v>6</v>
       </c>
       <c r="D49" s="14">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E49" s="14">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>298</v>
+        <v>151</v>
       </c>
       <c r="G49" s="14"/>
       <c r="H49" s="2"/>
@@ -2861,19 +2867,19 @@
         <v>7</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C50" s="14">
         <v>6</v>
       </c>
       <c r="D50" s="14">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E50" s="14">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>174</v>
+        <v>298</v>
       </c>
       <c r="G50" s="14"/>
       <c r="H50" s="2"/>
@@ -2883,19 +2889,19 @@
         <v>7</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>369</v>
+        <v>315</v>
       </c>
       <c r="C51" s="14">
         <v>6</v>
       </c>
       <c r="D51" s="14">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E51" s="14">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>370</v>
+        <v>174</v>
       </c>
       <c r="G51" s="14"/>
       <c r="H51" s="2"/>
@@ -2905,19 +2911,19 @@
         <v>7</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C52" s="14">
         <v>6</v>
       </c>
       <c r="D52" s="14">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E52" s="14">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>142</v>
+        <v>370</v>
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="2"/>
@@ -2927,65 +2933,65 @@
         <v>7</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C53" s="14">
         <v>6</v>
       </c>
       <c r="D53" s="14">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E53" s="14">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>376</v>
+        <v>142</v>
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="1">
-        <v>12</v>
-      </c>
-      <c r="D54" s="1">
-        <v>55</v>
-      </c>
-      <c r="E54" s="1">
-        <v>25</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G54" s="1"/>
+      <c r="A54" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C54" s="14">
+        <v>6</v>
+      </c>
+      <c r="D54" s="14">
+        <v>58</v>
+      </c>
+      <c r="E54" s="14">
+        <v>58</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="G54" s="14"/>
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C55" s="1">
-        <v>12</v>
-      </c>
-      <c r="D55" s="1">
-        <v>53</v>
-      </c>
-      <c r="E55" s="1">
-        <v>25</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G55" s="1"/>
+      <c r="A55" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C55" s="14">
+        <v>6</v>
+      </c>
+      <c r="D55" s="14">
+        <v>52</v>
+      </c>
+      <c r="E55" s="14">
+        <v>52</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G55" s="14"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2993,19 +2999,19 @@
         <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C56" s="1">
         <v>12</v>
       </c>
       <c r="D56" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E56" s="1">
         <v>25</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="2"/>
@@ -3015,19 +3021,19 @@
         <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C57" s="1">
         <v>12</v>
       </c>
       <c r="D57" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E57" s="1">
         <v>25</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="2"/>
@@ -3037,13 +3043,13 @@
         <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C58" s="1">
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E58" s="1">
         <v>25</v>
@@ -3059,19 +3065,19 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C59" s="1">
         <v>12</v>
       </c>
       <c r="D59" s="1">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E59" s="1">
         <v>25</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="2"/>
@@ -3081,19 +3087,19 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C60" s="1">
         <v>12</v>
       </c>
       <c r="D60" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E60" s="1">
         <v>25</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="2"/>
@@ -3103,19 +3109,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C61" s="1">
         <v>12</v>
       </c>
       <c r="D61" s="1">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E61" s="1">
         <v>25</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="2"/>
@@ -3125,19 +3131,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C62" s="1">
         <v>12</v>
       </c>
       <c r="D62" s="1">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E62" s="1">
         <v>25</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="2"/>
@@ -3147,19 +3153,19 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C63" s="1">
         <v>12</v>
       </c>
       <c r="D63" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E63" s="1">
         <v>25</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="2"/>
@@ -3169,62 +3175,86 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C64" s="1">
         <v>12</v>
       </c>
       <c r="D64" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E64" s="1">
         <v>25</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="C65" s="1">
         <v>12</v>
       </c>
       <c r="D65" s="1">
+        <v>55</v>
+      </c>
+      <c r="E65" s="1">
+        <v>25</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G65" s="1"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C66" s="1">
+        <v>12</v>
+      </c>
+      <c r="D66" s="1">
+        <v>53</v>
+      </c>
+      <c r="E66" s="1">
+        <v>25</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C67" s="1">
+        <v>12</v>
+      </c>
+      <c r="D67" s="1">
         <v>293</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E67" s="1">
         <v>137</v>
       </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="30"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
+      <c r="H67" s="30"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
@@ -3266,6 +3296,26 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3273,10 +3323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
-  <dimension ref="A1:T72"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView topLeftCell="B45" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4706,69 +4756,65 @@
       <c r="S33" s="14"/>
       <c r="T33" s="14"/>
     </row>
-    <row r="34" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1">
-        <v>727</v>
-      </c>
-      <c r="D35" s="1">
-        <v>100</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" s="18" t="s">
-        <v>22</v>
-      </c>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C34" s="14">
+        <v>910</v>
+      </c>
+      <c r="D34" s="14">
+        <v>94</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+    </row>
+    <row r="35" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="M35" s="36"/>
-      <c r="N35" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="O35" s="37"/>
-      <c r="P35" s="37"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -4779,38 +4825,42 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="1">
-        <v>505</v>
+        <v>727</v>
       </c>
       <c r="D36" s="1">
-        <v>84</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>26</v>
+        <v>100</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
+      <c r="L36" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="36"/>
+      <c r="N36" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -4821,31 +4871,31 @@
         <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1">
-        <v>535</v>
+        <v>505</v>
       </c>
       <c r="D37" s="1">
-        <v>50</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>36</v>
+        <v>84</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -4863,31 +4913,31 @@
         <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1">
-        <v>700</v>
+        <v>535</v>
       </c>
       <c r="D38" s="1">
-        <v>100</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J38" s="18" t="s">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -4901,245 +4951,245 @@
       <c r="T38" s="1"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="1">
+        <v>700</v>
+      </c>
+      <c r="D39" s="1">
+        <v>100</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C40" s="7">
         <v>669</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D40" s="7">
         <v>94</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F40" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="19" t="s">
+      <c r="H40" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I39" s="19" t="s">
+      <c r="I40" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="J39" s="16" t="s">
+      <c r="J40" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B41" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C41" s="9">
         <v>791</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D41" s="9">
         <v>98</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E41" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F41" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G41" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="H41" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I41" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J40" s="19" t="s">
+      <c r="J41" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B42" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C42" s="11">
         <v>853</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D42" s="11">
         <v>100</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F42" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G42" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H41" s="19" t="s">
+      <c r="H42" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I41" s="19" t="s">
+      <c r="I42" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="J41" s="17" t="s">
+      <c r="J42" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K41" s="8"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="K42" s="8"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B43" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C43" s="13">
         <v>740</v>
       </c>
-      <c r="D42" s="13">
+      <c r="D43" s="13">
         <v>90</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E43" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H42" s="22" t="s">
+      <c r="H43" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="I42" s="17" t="s">
+      <c r="I43" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="J43" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="13"/>
-      <c r="T42" s="13"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" s="14">
-        <v>848</v>
-      </c>
-      <c r="D43" s="14">
-        <v>100</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="J43" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K43" s="8"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C44" s="14">
-        <v>519</v>
+        <v>848</v>
       </c>
       <c r="D44" s="14">
         <v>100</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>92</v>
+        <v>17</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="J44" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44" s="14"/>
@@ -5157,31 +5207,31 @@
         <v>7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C45" s="14">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="D45" s="14">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I45" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J45" s="19" t="s">
-        <v>180</v>
+        <v>77</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="K45" s="8"/>
       <c r="L45" s="14"/>
@@ -5199,31 +5249,31 @@
         <v>7</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C46" s="14">
-        <v>595</v>
+        <v>503</v>
       </c>
       <c r="D46" s="14">
         <v>98</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G46" s="22" t="s">
+      <c r="F46" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H46" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="I46" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="J46" s="20" t="s">
-        <v>48</v>
+      <c r="G46" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="14"/>
@@ -5241,31 +5291,31 @@
         <v>7</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C47" s="14">
-        <v>573</v>
+        <v>595</v>
       </c>
       <c r="D47" s="14">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H47" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="I47" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I47" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="J47" s="17" t="s">
-        <v>172</v>
+      <c r="J47" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="K47" s="8"/>
       <c r="L47" s="14"/>
@@ -5283,44 +5333,40 @@
         <v>7</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C48" s="14">
-        <v>750</v>
+        <v>573</v>
       </c>
       <c r="D48" s="14">
         <v>100</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G48" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H48" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="I48" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J48" s="28" t="s">
-        <v>217</v>
+      <c r="H48" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="J48" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="K48" s="8"/>
-      <c r="L48" s="37" t="s">
-        <v>225</v>
-      </c>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="37"/>
-      <c r="Q48" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="R48" s="38"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
       <c r="S48" s="14"/>
       <c r="T48" s="14"/>
     </row>
@@ -5329,40 +5375,44 @@
         <v>7</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C49" s="14">
-        <v>534</v>
+        <v>750</v>
       </c>
       <c r="D49" s="14">
-        <v>46</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H49" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="J49" s="19" t="s">
-        <v>244</v>
+        <v>100</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I49" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J49" s="28" t="s">
+        <v>217</v>
       </c>
       <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
+      <c r="L49" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="R49" s="38"/>
       <c r="S49" s="14"/>
       <c r="T49" s="14"/>
     </row>
@@ -5371,31 +5421,31 @@
         <v>7</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="C50" s="14">
-        <v>830</v>
+        <v>534</v>
       </c>
       <c r="D50" s="14">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H50" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="I50" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="J50" s="35" t="s">
-        <v>292</v>
+        <v>240</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H50" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="J50" s="19" t="s">
+        <v>244</v>
       </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
@@ -5413,31 +5463,31 @@
         <v>7</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C51" s="14">
-        <v>818</v>
+        <v>830</v>
       </c>
       <c r="D51" s="14">
-        <v>68</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>299</v>
+        <v>98</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>268</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="H51" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="J51" s="17" t="s">
-        <v>303</v>
+        <v>25</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="J51" s="35" t="s">
+        <v>292</v>
       </c>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
@@ -5455,31 +5505,31 @@
         <v>7</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C52" s="14">
-        <v>794</v>
+        <v>818</v>
       </c>
       <c r="D52" s="14">
-        <v>86</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="G52" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="H52" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>285</v>
+      <c r="G52" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="J52" s="17" t="s">
+        <v>303</v>
       </c>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
@@ -5497,31 +5547,31 @@
         <v>7</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>369</v>
+        <v>315</v>
       </c>
       <c r="C53" s="14">
-        <v>455</v>
+        <v>794</v>
       </c>
       <c r="D53" s="14">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>206</v>
+        <v>18</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>97</v>
+        <v>299</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
       <c r="J53" s="8" t="s">
-        <v>371</v>
+        <v>285</v>
       </c>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
@@ -5539,31 +5589,31 @@
         <v>7</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C54" s="14">
-        <v>585</v>
+        <v>455</v>
       </c>
       <c r="D54" s="14">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>374</v>
+        <v>126</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>375</v>
+        <v>289</v>
       </c>
       <c r="J54" s="8" t="s">
-        <v>126</v>
+        <v>371</v>
       </c>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
@@ -5581,31 +5631,31 @@
         <v>7</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C55" s="14">
-        <v>661</v>
+        <v>585</v>
       </c>
       <c r="D55" s="14">
         <v>100</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>377</v>
+        <v>123</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>380</v>
+        <v>126</v>
       </c>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
@@ -5618,131 +5668,105 @@
       <c r="S55" s="14"/>
       <c r="T55" s="14"/>
     </row>
-    <row r="56" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="C56" s="14">
+        <v>661</v>
+      </c>
+      <c r="D56" s="14">
+        <v>100</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="14"/>
+      <c r="T56" s="14"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="1">
-        <v>2470</v>
-      </c>
-      <c r="D57" s="1">
-        <v>100</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G57" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H57" s="5" t="s">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C57" s="14">
+        <v>1136</v>
+      </c>
+      <c r="D57" s="14">
+        <v>98</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I57" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J57" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K57" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="L57" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M57" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N57" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O57" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P57" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-      <c r="S57" s="1"/>
-      <c r="T57" s="1"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1891</v>
-      </c>
-      <c r="D58" s="1">
-        <v>88</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I58" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="J58" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K58" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="L58" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M58" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N58" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="O58" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="P58" s="17" t="s">
-        <v>93</v>
-      </c>
+      <c r="G57" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="8"/>
+      <c r="S57" s="14"/>
+      <c r="T57" s="14"/>
+    </row>
+    <row r="58" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
@@ -5753,49 +5777,49 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C59" s="1">
-        <v>2256</v>
+        <v>2470</v>
       </c>
       <c r="D59" s="1">
         <v>100</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="G59" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>82</v>
+        <v>63</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="K59" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L59" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="M59" s="19" t="s">
-        <v>97</v>
+        <v>69</v>
+      </c>
+      <c r="K59" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L59" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M59" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="N59" s="18" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="O59" s="18" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="P59" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
@@ -5807,49 +5831,49 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C60" s="1">
-        <v>2654</v>
+        <v>1891</v>
       </c>
       <c r="D60" s="1">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>109</v>
+        <v>44</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H60" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H60" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I60" s="15" t="s">
-        <v>69</v>
+      <c r="I60" s="19" t="s">
+        <v>290</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K60" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L60" s="19" t="s">
-        <v>111</v>
+        <v>79</v>
+      </c>
+      <c r="L60" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="M60" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N60" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O60" s="19" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="N60" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O60" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="P60" s="17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -5861,49 +5885,49 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C61" s="1">
-        <v>2035</v>
+        <v>2256</v>
       </c>
       <c r="D61" s="1">
+        <v>100</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I61" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J61" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K61" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L61" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M61" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N61" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F61" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="H61" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="I61" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J61" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K61" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L61" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M61" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="N61" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="O61" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="P61" s="17" t="s">
-        <v>128</v>
+      <c r="O61" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="P61" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5915,49 +5939,49 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C62" s="1">
-        <v>2692</v>
+        <v>2654</v>
       </c>
       <c r="D62" s="1">
         <v>100</v>
       </c>
-      <c r="E62" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>83</v>
+      <c r="E62" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H62" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I62" s="16" t="s">
-        <v>143</v>
+        <v>110</v>
+      </c>
+      <c r="H62" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I62" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="J62" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K62" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L62" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M62" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K62" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="L62" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M62" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="N62" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="O62" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P62" s="18" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="O62" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="P62" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -5969,49 +5993,49 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C63" s="1">
-        <v>2216</v>
+        <v>2035</v>
       </c>
       <c r="D63" s="1">
-        <v>90</v>
-      </c>
-      <c r="E63" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H63" s="15" t="s">
-        <v>152</v>
+        <v>127</v>
+      </c>
+      <c r="H63" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="I63" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J63" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="K63" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L63" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="M63" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N63" s="17" t="s">
-        <v>157</v>
+        <v>84</v>
+      </c>
+      <c r="J63" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L63" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M63" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N63" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="O63" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="P63" s="16" t="s">
-        <v>92</v>
+        <v>111</v>
+      </c>
+      <c r="P63" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
@@ -6023,49 +6047,49 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C64" s="1">
-        <v>2066</v>
+        <v>2692</v>
       </c>
       <c r="D64" s="1">
         <v>100</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>179</v>
+        <v>83</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H64" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="I64" s="19" t="s">
-        <v>182</v>
+        <v>95</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I64" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="J64" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="K64" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L64" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="M64" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="N64" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="O64" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="P64" s="17" t="s">
-        <v>187</v>
+        <v>97</v>
+      </c>
+      <c r="K64" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L64" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M64" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="O64" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P64" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
@@ -6077,49 +6101,49 @@
         <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C65" s="1">
-        <v>2680</v>
+        <v>2216</v>
       </c>
       <c r="D65" s="1">
-        <v>100</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G65" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I65" s="22" t="s">
-        <v>197</v>
+        <v>90</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I65" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="J65" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K65" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="L65" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="M65" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N65" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="O65" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="P65" s="25" t="s">
-        <v>202</v>
+        <v>155</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L65" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="M65" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O65" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P65" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
@@ -6131,49 +6155,49 @@
         <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C66" s="1">
-        <v>1771</v>
+        <v>2066</v>
       </c>
       <c r="D66" s="1">
         <v>100</v>
       </c>
-      <c r="E66" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F66" s="22" t="s">
-        <v>42</v>
+      <c r="E66" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H66" s="16" t="s">
-        <v>206</v>
+        <v>110</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="I66" s="19" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="J66" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K66" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="L66" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="M66" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="N66" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O66" s="26" t="s">
-        <v>210</v>
+        <v>180</v>
+      </c>
+      <c r="K66" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L66" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="M66" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="N66" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="O66" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="P66" s="17" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
@@ -6185,49 +6209,49 @@
         <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C67" s="1">
-        <v>2700</v>
+        <v>2680</v>
       </c>
       <c r="D67" s="1">
         <v>100</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>215</v>
+        <v>52</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="G67" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H67" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="I67" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>167</v>
+      <c r="I67" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J67" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="L67" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M67" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="N67" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="O67" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="P67" s="27" t="s">
-        <v>224</v>
+        <v>126</v>
+      </c>
+      <c r="L67" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="M67" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="N67" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O67" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="P67" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
@@ -6235,22 +6259,54 @@
       <c r="T67" s="1"/>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1771</v>
+      </c>
+      <c r="D68" s="1">
+        <v>100</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I68" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J68" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K68" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L68" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M68" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="N68" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="O68" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="P68" s="17" t="s">
+        <v>196</v>
+      </c>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
@@ -6258,25 +6314,53 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="C69" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D69" s="1">
+        <v>100</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H69" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I69" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K69" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="L69" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M69" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="N69" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="O69" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="P69" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
@@ -6305,8 +6389,12 @@
       <c r="T70" s="1"/>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -6348,12 +6436,56 @@
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
     </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="L48:P48"/>
-    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="L49:P49"/>
+    <mergeCell ref="Q49:R49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Paris Roubaix M and F results
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1679" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C24772-63F4-423A-B996-4EA2EF480E6E}"/>
+  <xr:revisionPtr revIDLastSave="1720" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6091FCBC-E28E-476D-B4D5-C93BE9F7BE75}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="388">
   <si>
     <t>Type</t>
   </si>
@@ -1184,6 +1184,21 @@
   </si>
   <si>
     <t>Michael Valgren</t>
+  </si>
+  <si>
+    <t>Paris Roubaix</t>
+  </si>
+  <si>
+    <t>Franziska Koch</t>
+  </si>
+  <si>
+    <t>Heinrich Haussler</t>
+  </si>
+  <si>
+    <t>Florian Vermeersch</t>
+  </si>
+  <si>
+    <t>Guillaume Boivin</t>
   </si>
 </sst>
 </file>
@@ -1771,10 +1786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,25 +2526,25 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="A34" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C34" s="14">
         <v>6</v>
       </c>
-      <c r="D34" s="1">
-        <v>50</v>
-      </c>
-      <c r="E34" s="1">
-        <v>50</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="1"/>
+      <c r="D34" s="14">
+        <v>35</v>
+      </c>
+      <c r="E34" s="14">
+        <v>35</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="G34" s="14"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2537,19 +2552,19 @@
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35" s="1">
         <v>6</v>
       </c>
       <c r="D35" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E35" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
@@ -2559,19 +2574,19 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="1">
         <v>6</v>
       </c>
       <c r="D36" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E36" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="2"/>
@@ -2581,131 +2596,131 @@
         <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1">
         <v>6</v>
       </c>
       <c r="D37" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E37" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="1">
+        <v>6</v>
+      </c>
+      <c r="D38" s="1">
+        <v>55</v>
+      </c>
+      <c r="E38" s="1">
+        <v>55</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C39" s="7">
         <v>6</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D39" s="7">
         <v>53</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E39" s="7">
         <v>53</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="G39" s="7"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C40" s="9">
         <v>6</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D40" s="9">
         <v>45</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E40" s="9">
         <v>45</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F40" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="G40" s="9"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B41" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C41" s="11">
         <v>6</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D41" s="11">
         <v>44</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E41" s="11">
         <v>44</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F41" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="G41" s="11"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B42" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C42" s="12">
         <v>6</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D42" s="12">
         <v>47</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E42" s="12">
         <v>47</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F42" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C42" s="14">
-        <v>6</v>
-      </c>
-      <c r="D42" s="14">
-        <v>52</v>
-      </c>
-      <c r="E42" s="14">
-        <v>52</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="G42" s="14"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2713,19 +2728,19 @@
         <v>7</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C43" s="14">
         <v>6</v>
       </c>
       <c r="D43" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E43" s="14">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="G43" s="14"/>
       <c r="H43" s="2"/>
@@ -2735,19 +2750,19 @@
         <v>7</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C44" s="14">
         <v>6</v>
       </c>
       <c r="D44" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E44" s="14">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="2"/>
@@ -2757,19 +2772,19 @@
         <v>7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C45" s="14">
         <v>6</v>
       </c>
       <c r="D45" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E45" s="14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="G45" s="14"/>
       <c r="H45" s="2"/>
@@ -2779,7 +2794,7 @@
         <v>7</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C46" s="14">
         <v>6</v>
@@ -2801,19 +2816,19 @@
         <v>7</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C47" s="14">
         <v>6</v>
       </c>
       <c r="D47" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E47" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="G47" s="14"/>
       <c r="H47" s="2"/>
@@ -2823,19 +2838,19 @@
         <v>7</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C48" s="14">
         <v>6</v>
       </c>
       <c r="D48" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E48" s="14">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>132</v>
+        <v>214</v>
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="2"/>
@@ -2845,19 +2860,19 @@
         <v>7</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="C49" s="14">
         <v>6</v>
       </c>
       <c r="D49" s="14">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E49" s="14">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="G49" s="14"/>
       <c r="H49" s="2"/>
@@ -2867,19 +2882,19 @@
         <v>7</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C50" s="14">
         <v>6</v>
       </c>
       <c r="D50" s="14">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E50" s="14">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>298</v>
+        <v>151</v>
       </c>
       <c r="G50" s="14"/>
       <c r="H50" s="2"/>
@@ -2889,19 +2904,19 @@
         <v>7</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C51" s="14">
         <v>6</v>
       </c>
       <c r="D51" s="14">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E51" s="14">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>174</v>
+        <v>298</v>
       </c>
       <c r="G51" s="14"/>
       <c r="H51" s="2"/>
@@ -2911,19 +2926,19 @@
         <v>7</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>369</v>
+        <v>315</v>
       </c>
       <c r="C52" s="14">
         <v>6</v>
       </c>
       <c r="D52" s="14">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E52" s="14">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>370</v>
+        <v>174</v>
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="2"/>
@@ -2933,19 +2948,19 @@
         <v>7</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C53" s="14">
         <v>6</v>
       </c>
       <c r="D53" s="14">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E53" s="14">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>142</v>
+        <v>370</v>
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="2"/>
@@ -2955,19 +2970,19 @@
         <v>7</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C54" s="14">
         <v>6</v>
       </c>
       <c r="D54" s="14">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E54" s="14">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>376</v>
+        <v>142</v>
       </c>
       <c r="G54" s="14"/>
       <c r="H54" s="2"/>
@@ -2977,65 +2992,65 @@
         <v>7</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C55" s="14">
         <v>6</v>
       </c>
       <c r="D55" s="14">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E55" s="14">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="G55" s="14"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="1">
-        <v>12</v>
-      </c>
-      <c r="D56" s="1">
-        <v>55</v>
-      </c>
-      <c r="E56" s="1">
-        <v>25</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G56" s="1"/>
+      <c r="A56" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C56" s="14">
+        <v>6</v>
+      </c>
+      <c r="D56" s="14">
+        <v>52</v>
+      </c>
+      <c r="E56" s="14">
+        <v>52</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G56" s="14"/>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="1">
-        <v>12</v>
-      </c>
-      <c r="D57" s="1">
-        <v>53</v>
-      </c>
-      <c r="E57" s="1">
-        <v>25</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G57" s="1"/>
+      <c r="A57" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C57" s="14">
+        <v>6</v>
+      </c>
+      <c r="D57" s="14">
+        <v>47</v>
+      </c>
+      <c r="E57" s="14">
+        <v>47</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G57" s="14"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3043,19 +3058,19 @@
         <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C58" s="1">
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E58" s="1">
         <v>25</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="2"/>
@@ -3065,19 +3080,19 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C59" s="1">
         <v>12</v>
       </c>
       <c r="D59" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E59" s="1">
         <v>25</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="2"/>
@@ -3087,13 +3102,13 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C60" s="1">
         <v>12</v>
       </c>
       <c r="D60" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E60" s="1">
         <v>25</v>
@@ -3109,19 +3124,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C61" s="1">
         <v>12</v>
       </c>
       <c r="D61" s="1">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E61" s="1">
         <v>25</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="2"/>
@@ -3131,19 +3146,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C62" s="1">
         <v>12</v>
       </c>
       <c r="D62" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E62" s="1">
         <v>25</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="2"/>
@@ -3153,19 +3168,19 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C63" s="1">
         <v>12</v>
       </c>
       <c r="D63" s="1">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E63" s="1">
         <v>25</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="2"/>
@@ -3175,19 +3190,19 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C64" s="1">
         <v>12</v>
       </c>
       <c r="D64" s="1">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E64" s="1">
         <v>25</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="2"/>
@@ -3197,19 +3212,19 @@
         <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C65" s="1">
         <v>12</v>
       </c>
       <c r="D65" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E65" s="1">
         <v>25</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="2"/>
@@ -3219,62 +3234,86 @@
         <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C66" s="1">
         <v>12</v>
       </c>
       <c r="D66" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E66" s="1">
         <v>25</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="C67" s="1">
         <v>12</v>
       </c>
       <c r="D67" s="1">
+        <v>55</v>
+      </c>
+      <c r="E67" s="1">
+        <v>25</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G67" s="1"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C68" s="1">
+        <v>12</v>
+      </c>
+      <c r="D68" s="1">
+        <v>53</v>
+      </c>
+      <c r="E68" s="1">
+        <v>25</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G68" s="1"/>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C69" s="1">
+        <v>12</v>
+      </c>
+      <c r="D69" s="1">
         <v>293</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E69" s="1">
         <v>137</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="30"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
+      <c r="H69" s="30"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
@@ -3316,6 +3355,26 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3323,10 +3382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
-  <dimension ref="A1:T74"/>
+  <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4798,69 +4857,65 @@
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
     </row>
-    <row r="35" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="1">
-        <v>727</v>
-      </c>
-      <c r="D36" s="1">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C35" s="14">
+        <v>925</v>
+      </c>
+      <c r="D35" s="14">
         <v>100</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>22</v>
-      </c>
+      <c r="E35" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="K35" s="14"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+    </row>
+    <row r="36" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="M36" s="36"/>
-      <c r="N36" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -4871,38 +4926,42 @@
         <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="1">
-        <v>505</v>
+        <v>727</v>
       </c>
       <c r="D37" s="1">
-        <v>84</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>26</v>
+        <v>100</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="I37" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+      <c r="L37" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M37" s="36"/>
+      <c r="N37" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -4913,31 +4972,31 @@
         <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" s="1">
-        <v>535</v>
+        <v>505</v>
       </c>
       <c r="D38" s="1">
-        <v>50</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>36</v>
+        <v>84</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -4955,31 +5014,31 @@
         <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1">
-        <v>700</v>
+        <v>535</v>
       </c>
       <c r="D39" s="1">
-        <v>100</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H39" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="J39" s="18" t="s">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -4993,245 +5052,245 @@
       <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="1">
+        <v>700</v>
+      </c>
+      <c r="D40" s="1">
+        <v>100</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J40" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C41" s="7">
         <v>669</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D41" s="7">
         <v>94</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F41" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="H41" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I41" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="J40" s="16" t="s">
+      <c r="J41" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C42" s="9">
         <v>791</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D42" s="9">
         <v>98</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E42" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F42" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G41" s="22" t="s">
+      <c r="G42" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H41" s="19" t="s">
+      <c r="H42" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I41" s="19" t="s">
+      <c r="I42" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="J42" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-      <c r="T41" s="9"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C43" s="11">
         <v>853</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D43" s="11">
         <v>100</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F43" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G43" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="H43" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I42" s="19" t="s">
+      <c r="I43" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="J42" s="17" t="s">
+      <c r="J43" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K42" s="8"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="K43" s="8"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B44" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C44" s="13">
         <v>740</v>
       </c>
-      <c r="D43" s="13">
+      <c r="D44" s="13">
         <v>90</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E44" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H43" s="22" t="s">
+      <c r="H44" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="I43" s="17" t="s">
+      <c r="I44" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J44" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="13"/>
-      <c r="S43" s="13"/>
-      <c r="T43" s="13"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="14">
-        <v>848</v>
-      </c>
-      <c r="D44" s="14">
-        <v>100</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H44" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="J44" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K44" s="8"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-      <c r="T44" s="14"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C45" s="14">
-        <v>519</v>
+        <v>848</v>
       </c>
       <c r="D45" s="14">
         <v>100</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>92</v>
+        <v>17</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="J45" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="K45" s="8"/>
       <c r="L45" s="14"/>
@@ -5249,31 +5308,31 @@
         <v>7</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C46" s="14">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="D46" s="14">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J46" s="19" t="s">
-        <v>180</v>
+        <v>77</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="14"/>
@@ -5291,31 +5350,31 @@
         <v>7</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C47" s="14">
-        <v>595</v>
+        <v>503</v>
       </c>
       <c r="D47" s="14">
         <v>98</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G47" s="22" t="s">
+      <c r="F47" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H47" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="I47" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="J47" s="20" t="s">
-        <v>48</v>
+      <c r="G47" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J47" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="K47" s="8"/>
       <c r="L47" s="14"/>
@@ -5333,31 +5392,31 @@
         <v>7</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C48" s="14">
-        <v>573</v>
+        <v>595</v>
       </c>
       <c r="D48" s="14">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H48" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="I48" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I48" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="J48" s="17" t="s">
-        <v>172</v>
+      <c r="J48" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="K48" s="8"/>
       <c r="L48" s="14"/>
@@ -5375,44 +5434,40 @@
         <v>7</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C49" s="14">
-        <v>750</v>
+        <v>573</v>
       </c>
       <c r="D49" s="14">
         <v>100</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G49" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="I49" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J49" s="28" t="s">
-        <v>217</v>
+      <c r="H49" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="I49" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="J49" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="K49" s="8"/>
-      <c r="L49" s="37" t="s">
-        <v>225</v>
-      </c>
-      <c r="M49" s="37"/>
-      <c r="N49" s="37"/>
-      <c r="O49" s="37"/>
-      <c r="P49" s="37"/>
-      <c r="Q49" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="R49" s="38"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
       <c r="S49" s="14"/>
       <c r="T49" s="14"/>
     </row>
@@ -5421,40 +5476,44 @@
         <v>7</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C50" s="14">
-        <v>534</v>
+        <v>750</v>
       </c>
       <c r="D50" s="14">
-        <v>46</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="I50" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="J50" s="19" t="s">
-        <v>244</v>
+        <v>100</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I50" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J50" s="28" t="s">
+        <v>217</v>
       </c>
       <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
+      <c r="L50" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="R50" s="38"/>
       <c r="S50" s="14"/>
       <c r="T50" s="14"/>
     </row>
@@ -5463,31 +5522,31 @@
         <v>7</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="C51" s="14">
-        <v>830</v>
+        <v>534</v>
       </c>
       <c r="D51" s="14">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="J51" s="35" t="s">
-        <v>292</v>
+        <v>240</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H51" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="I51" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="J51" s="19" t="s">
+        <v>244</v>
       </c>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
@@ -5505,31 +5564,31 @@
         <v>7</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C52" s="14">
-        <v>818</v>
+        <v>830</v>
       </c>
       <c r="D52" s="14">
-        <v>68</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>299</v>
+        <v>98</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>268</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="J52" s="17" t="s">
-        <v>303</v>
+        <v>25</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="J52" s="35" t="s">
+        <v>292</v>
       </c>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
@@ -5547,31 +5606,31 @@
         <v>7</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C53" s="14">
-        <v>794</v>
+        <v>818</v>
       </c>
       <c r="D53" s="14">
-        <v>86</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="G53" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="H53" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I53" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>285</v>
+      <c r="G53" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="J53" s="17" t="s">
+        <v>303</v>
       </c>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
@@ -5589,31 +5648,31 @@
         <v>7</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>369</v>
+        <v>315</v>
       </c>
       <c r="C54" s="14">
-        <v>455</v>
+        <v>794</v>
       </c>
       <c r="D54" s="14">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>206</v>
+        <v>18</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>97</v>
+        <v>299</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
       <c r="J54" s="8" t="s">
-        <v>371</v>
+        <v>285</v>
       </c>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
@@ -5631,31 +5690,31 @@
         <v>7</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C55" s="14">
-        <v>585</v>
+        <v>455</v>
       </c>
       <c r="D55" s="14">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>374</v>
+        <v>126</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>375</v>
+        <v>289</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>126</v>
+        <v>371</v>
       </c>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
@@ -5673,31 +5732,31 @@
         <v>7</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C56" s="14">
-        <v>661</v>
+        <v>585</v>
       </c>
       <c r="D56" s="14">
         <v>100</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>377</v>
+        <v>123</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J56" s="8" t="s">
-        <v>380</v>
+        <v>126</v>
       </c>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
@@ -5711,33 +5770,35 @@
       <c r="T56" s="14"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="B57" s="14" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C57" s="14">
-        <v>1136</v>
+        <v>661</v>
       </c>
       <c r="D57" s="14">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>64</v>
+        <v>377</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>302</v>
+        <v>379</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>87</v>
+        <v>380</v>
       </c>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
@@ -5750,131 +5811,107 @@
       <c r="S57" s="14"/>
       <c r="T57" s="14"/>
     </row>
-    <row r="58" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-      <c r="T58" s="1"/>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C58" s="14">
+        <v>1136</v>
+      </c>
+      <c r="D58" s="14">
+        <v>98</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="J58" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="14"/>
+      <c r="T58" s="14"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="1">
-        <v>2470</v>
-      </c>
-      <c r="D59" s="1">
-        <v>100</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F59" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G59" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I59" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J59" s="19" t="s">
+      <c r="A59" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C59" s="14">
+        <v>1005</v>
+      </c>
+      <c r="D59" s="14">
+        <v>96</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="G59" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K59" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="L59" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M59" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N59" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O59" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P59" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-      <c r="T59" s="1"/>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1891</v>
-      </c>
-      <c r="D60" s="1">
-        <v>88</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F60" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I60" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="J60" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K60" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="L60" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M60" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N60" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="O60" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="P60" s="17" t="s">
-        <v>93</v>
-      </c>
+      <c r="H59" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="8"/>
+      <c r="S59" s="14"/>
+      <c r="T59" s="14"/>
+    </row>
+    <row r="60" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
@@ -5885,49 +5922,49 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C61" s="1">
-        <v>2256</v>
+        <v>2470</v>
       </c>
       <c r="D61" s="1">
         <v>100</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="G61" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>82</v>
+        <v>63</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="K61" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L61" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="M61" s="19" t="s">
-        <v>97</v>
+        <v>69</v>
+      </c>
+      <c r="K61" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L61" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M61" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="N61" s="18" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="O61" s="18" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="P61" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5939,49 +5976,49 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C62" s="1">
-        <v>2654</v>
+        <v>1891</v>
       </c>
       <c r="D62" s="1">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>109</v>
+        <v>44</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H62" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H62" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I62" s="15" t="s">
-        <v>69</v>
+      <c r="I62" s="19" t="s">
+        <v>290</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K62" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L62" s="19" t="s">
-        <v>111</v>
+        <v>79</v>
+      </c>
+      <c r="L62" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="M62" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N62" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O62" s="19" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="N62" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O62" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="P62" s="17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -5993,49 +6030,49 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="C63" s="1">
-        <v>2035</v>
+        <v>2256</v>
       </c>
       <c r="D63" s="1">
+        <v>100</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G63" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I63" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J63" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K63" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L63" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M63" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N63" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G63" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="H63" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="I63" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J63" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K63" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L63" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M63" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="N63" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="O63" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="P63" s="17" t="s">
-        <v>128</v>
+      <c r="O63" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="P63" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
@@ -6047,49 +6084,49 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C64" s="1">
-        <v>2692</v>
+        <v>2654</v>
       </c>
       <c r="D64" s="1">
         <v>100</v>
       </c>
-      <c r="E64" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>83</v>
+      <c r="E64" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H64" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>143</v>
+        <v>110</v>
+      </c>
+      <c r="H64" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I64" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="J64" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K64" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L64" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M64" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K64" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="L64" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M64" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="N64" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="O64" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P64" s="18" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="O64" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="P64" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
@@ -6101,49 +6138,49 @@
         <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C65" s="1">
-        <v>2216</v>
+        <v>2035</v>
       </c>
       <c r="D65" s="1">
-        <v>90</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>77</v>
+        <v>98</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>152</v>
+        <v>127</v>
+      </c>
+      <c r="H65" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="I65" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J65" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="K65" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L65" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="M65" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N65" s="17" t="s">
-        <v>157</v>
+        <v>84</v>
+      </c>
+      <c r="J65" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L65" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M65" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N65" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="O65" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="P65" s="16" t="s">
-        <v>92</v>
+        <v>111</v>
+      </c>
+      <c r="P65" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
@@ -6155,49 +6192,49 @@
         <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C66" s="1">
-        <v>2066</v>
+        <v>2692</v>
       </c>
       <c r="D66" s="1">
         <v>100</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>179</v>
+        <v>83</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H66" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="I66" s="19" t="s">
-        <v>182</v>
+        <v>95</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I66" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="J66" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="K66" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L66" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="M66" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="N66" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="O66" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="P66" s="17" t="s">
-        <v>187</v>
+        <v>97</v>
+      </c>
+      <c r="K66" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L66" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M66" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="N66" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="O66" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P66" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
@@ -6209,49 +6246,49 @@
         <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C67" s="1">
-        <v>2680</v>
+        <v>2216</v>
       </c>
       <c r="D67" s="1">
-        <v>100</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G67" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>197</v>
+        <v>90</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G67" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I67" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="J67" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K67" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="L67" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="M67" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N67" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="O67" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="P67" s="25" t="s">
-        <v>202</v>
+        <v>155</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L67" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="M67" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N67" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O67" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P67" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
@@ -6263,49 +6300,49 @@
         <v>60</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="C68" s="1">
-        <v>1771</v>
+        <v>2066</v>
       </c>
       <c r="D68" s="1">
         <v>100</v>
       </c>
-      <c r="E68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F68" s="22" t="s">
-        <v>42</v>
+      <c r="E68" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>206</v>
+        <v>110</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="I68" s="19" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="J68" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K68" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="L68" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="M68" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="N68" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O68" s="26" t="s">
-        <v>210</v>
+        <v>180</v>
+      </c>
+      <c r="K68" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L68" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="M68" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="N68" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="O68" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="P68" s="17" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
@@ -6317,49 +6354,49 @@
         <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C69" s="1">
-        <v>2700</v>
+        <v>2680</v>
       </c>
       <c r="D69" s="1">
         <v>100</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F69" s="17" t="s">
-        <v>215</v>
+        <v>52</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="G69" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H69" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H69" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="I69" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>167</v>
+      <c r="I69" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J69" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="K69" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="L69" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M69" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="N69" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="O69" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="P69" s="27" t="s">
-        <v>224</v>
+        <v>126</v>
+      </c>
+      <c r="L69" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="M69" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="N69" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O69" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="P69" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
@@ -6367,22 +6404,54 @@
       <c r="T69" s="1"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
+      <c r="A70" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1771</v>
+      </c>
+      <c r="D70" s="1">
+        <v>100</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H70" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I70" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J70" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K70" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L70" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M70" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="N70" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="O70" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="P70" s="17" t="s">
+        <v>196</v>
+      </c>
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
@@ -6390,25 +6459,53 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D71" s="1">
+        <v>100</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H71" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I71" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K71" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="L71" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M71" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="N71" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="O71" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="P71" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
@@ -6437,8 +6534,12 @@
       <c r="T72" s="1"/>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -6480,12 +6581,56 @@
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
     </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N36:P36"/>
-    <mergeCell ref="L49:P49"/>
-    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="L50:P50"/>
+    <mergeCell ref="Q50:R50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with CB, TVV, MT, GP results
</commit_message>
<xml_diff>
--- a/VUT_2021.xlsx
+++ b/VUT_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1720" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6091FCBC-E28E-476D-B4D5-C93BE9F7BE75}"/>
+  <xr:revisionPtr revIDLastSave="1792" documentId="8_{1C7F7B55-C055-453F-B037-80740CF9BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B51700B-A15A-4F31-9100-60867E18955E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ADF7A67D-4B9D-435F-A715-C9A322FA6B3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="404">
   <si>
     <t>Type</t>
   </si>
@@ -1199,6 +1199,54 @@
   </si>
   <si>
     <t>Guillaume Boivin</t>
+  </si>
+  <si>
+    <t>Coppa Bernocchi</t>
+  </si>
+  <si>
+    <t>Tre Valli Varesine</t>
+  </si>
+  <si>
+    <t>Milano Torino</t>
+  </si>
+  <si>
+    <t>3''</t>
+  </si>
+  <si>
+    <t>Remco Evenepoel</t>
+  </si>
+  <si>
+    <t>Thibaut Pinot</t>
+  </si>
+  <si>
+    <t>Samuele Battistella</t>
+  </si>
+  <si>
+    <t>Juan Sebastian Molano</t>
+  </si>
+  <si>
+    <t>Davide Formolo</t>
+  </si>
+  <si>
+    <t>Alessandro De Marchi</t>
+  </si>
+  <si>
+    <t>Nelson Oliveira</t>
+  </si>
+  <si>
+    <t>Gran Piemonte</t>
+  </si>
+  <si>
+    <t>Jakub Marezcko</t>
+  </si>
+  <si>
+    <t>Olav Kooij</t>
+  </si>
+  <si>
+    <t>Biniam Ghirmay</t>
+  </si>
+  <si>
+    <t>Matthew Halls</t>
   </si>
 </sst>
 </file>
@@ -1786,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA14938D-83E3-4863-A48D-E2F5F7761598}">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,91 +3102,91 @@
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" s="1">
-        <v>12</v>
-      </c>
-      <c r="D58" s="1">
-        <v>55</v>
-      </c>
-      <c r="E58" s="1">
-        <v>25</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G58" s="1"/>
+      <c r="A58" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C58" s="14">
+        <v>6</v>
+      </c>
+      <c r="D58" s="14">
+        <v>34</v>
+      </c>
+      <c r="E58" s="14">
+        <v>34</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="G58" s="14"/>
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C59" s="1">
-        <v>12</v>
-      </c>
-      <c r="D59" s="1">
-        <v>53</v>
-      </c>
-      <c r="E59" s="1">
-        <v>25</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G59" s="1"/>
+      <c r="A59" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C59" s="14">
+        <v>6</v>
+      </c>
+      <c r="D59" s="14">
+        <v>40</v>
+      </c>
+      <c r="E59" s="14">
+        <v>40</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="G59" s="14"/>
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" s="1">
-        <v>12</v>
-      </c>
-      <c r="D60" s="1">
+      <c r="A60" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C60" s="14">
+        <v>6</v>
+      </c>
+      <c r="D60" s="14">
+        <v>46</v>
+      </c>
+      <c r="E60" s="14">
+        <v>46</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="G60" s="14"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="C61" s="14">
+        <v>6</v>
+      </c>
+      <c r="D61" s="14">
         <v>45</v>
       </c>
-      <c r="E60" s="1">
-        <v>25</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="E61" s="14">
+        <v>45</v>
+      </c>
+      <c r="F61" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" s="1">
-        <v>12</v>
-      </c>
-      <c r="D61" s="1">
-        <v>44</v>
-      </c>
-      <c r="E61" s="1">
-        <v>25</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G61" s="1"/>
+      <c r="G61" s="14"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3146,19 +3194,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="C62" s="1">
         <v>12</v>
       </c>
       <c r="D62" s="1">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E62" s="1">
         <v>25</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="2"/>
@@ -3168,19 +3216,19 @@
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="C63" s="1">
         <v>12</v>
       </c>
       <c r="D63" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E63" s="1">
         <v>25</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="2"/>
@@ -3190,19 +3238,19 @@
         <v>60</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C64" s="1">
         <v>12</v>
       </c>
       <c r="D64" s="1">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E64" s="1">
         <v>25</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="2"/>
@@ -3212,13 +3260,13 @@
         <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>173</v>
+        <v>104</v>
       </c>
       <c r="C65" s="1">
         <v>12</v>
       </c>
       <c r="D65" s="1">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E65" s="1">
         <v>25</v>
@@ -3234,19 +3282,19 @@
         <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>188</v>
+        <v>122</v>
       </c>
       <c r="C66" s="1">
         <v>12</v>
       </c>
       <c r="D66" s="1">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E66" s="1">
         <v>25</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="2"/>
@@ -3256,19 +3304,19 @@
         <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>203</v>
+        <v>129</v>
       </c>
       <c r="C67" s="1">
         <v>12</v>
       </c>
       <c r="D67" s="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E67" s="1">
         <v>25</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>89</v>
+        <v>142</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="2"/>
@@ -3278,82 +3326,130 @@
         <v>60</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="C68" s="1">
         <v>12</v>
       </c>
       <c r="D68" s="1">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E68" s="1">
         <v>25</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>218</v>
+        <v>154</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>230</v>
+        <v>173</v>
       </c>
       <c r="C69" s="1">
         <v>12</v>
       </c>
       <c r="D69" s="1">
+        <v>56</v>
+      </c>
+      <c r="E69" s="1">
+        <v>25</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="1">
+        <v>12</v>
+      </c>
+      <c r="D70" s="1">
+        <v>55</v>
+      </c>
+      <c r="E70" s="1">
+        <v>25</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C71" s="1">
+        <v>12</v>
+      </c>
+      <c r="D71" s="1">
+        <v>55</v>
+      </c>
+      <c r="E71" s="1">
+        <v>25</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G71" s="1"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C72" s="1">
+        <v>12</v>
+      </c>
+      <c r="D72" s="1">
+        <v>53</v>
+      </c>
+      <c r="E72" s="1">
+        <v>25</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G72" s="1"/>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" s="1">
+        <v>12</v>
+      </c>
+      <c r="D73" s="1">
         <v>293</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E73" s="1">
         <v>137</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="30"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
+      <c r="H73" s="30"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
@@ -3375,6 +3471,46 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3382,10 +3518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DD095-D918-4A5B-8808-8FF5FBDD525F}">
-  <dimension ref="A1:T76"/>
+  <dimension ref="A1:T80"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5895,239 +6031,191 @@
       <c r="S59" s="14"/>
       <c r="T59" s="14"/>
     </row>
-    <row r="60" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-      <c r="T60" s="1"/>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C60" s="14">
+        <v>601</v>
+      </c>
+      <c r="D60" s="14">
+        <v>94</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="14"/>
+      <c r="T60" s="14"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="1">
-        <v>2470</v>
-      </c>
-      <c r="D61" s="1">
+      <c r="A61" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C61" s="14">
+        <v>616</v>
+      </c>
+      <c r="D61" s="14">
+        <v>86</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="14"/>
+      <c r="T61" s="14"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="C62" s="14">
+        <v>416</v>
+      </c>
+      <c r="D62" s="14">
         <v>100</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F61" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G61" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I61" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J61" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K61" s="18" t="s">
+      <c r="E62" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="I62" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="8"/>
+      <c r="R62" s="8"/>
+      <c r="S62" s="14"/>
+      <c r="T62" s="14"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="C63" s="14">
+        <v>455</v>
+      </c>
+      <c r="D63" s="14">
         <v>70</v>
       </c>
-      <c r="L61" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M61" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N61" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O61" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="P61" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-      <c r="T61" s="1"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1891</v>
-      </c>
-      <c r="D62" s="1">
-        <v>88</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F62" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H62" s="15" t="s">
+      <c r="E63" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I62" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="J62" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="K62" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="L62" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M62" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="N62" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="O62" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="P62" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="1">
-        <v>2256</v>
-      </c>
-      <c r="D63" s="1">
-        <v>100</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G63" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H63" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I63" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="J63" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="K63" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L63" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="M63" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N63" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="O63" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="P63" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" s="1">
-        <v>2654</v>
-      </c>
-      <c r="D64" s="1">
-        <v>100</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H64" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I64" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="J64" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="K64" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L64" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="M64" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N64" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="O64" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="P64" s="17" t="s">
-        <v>108</v>
-      </c>
+      <c r="G63" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="I63" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="14"/>
+      <c r="T63" s="14"/>
+    </row>
+    <row r="64" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
@@ -6138,49 +6226,49 @@
         <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="C65" s="1">
-        <v>2035</v>
+        <v>2470</v>
       </c>
       <c r="D65" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="H65" s="19" t="s">
-        <v>95</v>
+        <v>62</v>
+      </c>
+      <c r="G65" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I65" s="19" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="J65" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="K65" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="L65" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M65" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="N65" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="O65" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="P65" s="17" t="s">
-        <v>128</v>
+        <v>69</v>
+      </c>
+      <c r="K65" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L65" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M65" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="N65" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="O65" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="P65" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
@@ -6192,49 +6280,49 @@
         <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="C66" s="1">
-        <v>2692</v>
+        <v>1891</v>
       </c>
       <c r="D66" s="1">
-        <v>100</v>
-      </c>
-      <c r="E66" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I66" s="16" t="s">
-        <v>143</v>
+        <v>90</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>290</v>
       </c>
       <c r="J66" s="19" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="K66" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="L66" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M66" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="N66" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="O66" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="P66" s="18" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="L66" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="M66" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N66" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O66" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="P66" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
@@ -6246,49 +6334,49 @@
         <v>60</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="C67" s="1">
-        <v>2216</v>
+        <v>2256</v>
       </c>
       <c r="D67" s="1">
-        <v>90</v>
-      </c>
-      <c r="E67" s="22" t="s">
-        <v>44</v>
+        <v>100</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G67" s="19" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="I67" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J67" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="K67" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L67" s="17" t="s">
-        <v>156</v>
+        <v>95</v>
+      </c>
+      <c r="J67" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K67" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L67" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="M67" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N67" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="O67" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="P67" s="16" t="s">
-        <v>92</v>
+        <v>97</v>
+      </c>
+      <c r="N67" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="O67" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="P67" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
@@ -6300,49 +6388,49 @@
         <v>60</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>173</v>
+        <v>104</v>
       </c>
       <c r="C68" s="1">
-        <v>2066</v>
+        <v>2654</v>
       </c>
       <c r="D68" s="1">
         <v>100</v>
       </c>
-      <c r="E68" s="22" t="s">
+      <c r="E68" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F68" s="5" t="s">
-        <v>179</v>
+      <c r="F68" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="H68" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="I68" s="19" t="s">
-        <v>182</v>
+      <c r="H68" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I68" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="J68" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="K68" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L68" s="16" t="s">
-        <v>183</v>
+        <v>106</v>
+      </c>
+      <c r="K68" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L68" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="M68" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="N68" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="O68" s="17" t="s">
-        <v>186</v>
+        <v>97</v>
+      </c>
+      <c r="N68" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="O68" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="P68" s="17" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
@@ -6354,49 +6442,49 @@
         <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>188</v>
+        <v>122</v>
       </c>
       <c r="C69" s="1">
-        <v>2680</v>
+        <v>2035</v>
       </c>
       <c r="D69" s="1">
-        <v>100</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G69" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H69" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="J69" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K69" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I69" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="J69" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L69" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M69" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N69" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="L69" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="M69" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="N69" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="O69" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="P69" s="25" t="s">
-        <v>202</v>
+      <c r="O69" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="P69" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
@@ -6408,49 +6496,49 @@
         <v>60</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>203</v>
+        <v>129</v>
       </c>
       <c r="C70" s="1">
-        <v>1771</v>
+        <v>2692</v>
       </c>
       <c r="D70" s="1">
         <v>100</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70" s="22" t="s">
-        <v>42</v>
+      <c r="E70" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="I70" s="19" t="s">
-        <v>167</v>
+        <v>95</v>
+      </c>
+      <c r="H70" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I70" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="J70" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K70" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="L70" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="M70" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="N70" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O70" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="P70" s="17" t="s">
-        <v>196</v>
+        <v>97</v>
+      </c>
+      <c r="K70" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L70" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M70" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="N70" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="O70" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P70" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
@@ -6462,49 +6550,49 @@
         <v>60</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="C71" s="1">
-        <v>2700</v>
+        <v>2216</v>
       </c>
       <c r="D71" s="1">
-        <v>100</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F71" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="G71" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="I71" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="K71" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="L71" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="M71" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="N71" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="O71" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="P71" s="27" t="s">
-        <v>224</v>
+        <v>90</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H71" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="J71" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L71" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="M71" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N71" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O71" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P71" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
@@ -6512,22 +6600,54 @@
       <c r="T71" s="1"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2066</v>
+      </c>
+      <c r="D72" s="1">
+        <v>100</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H72" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="I72" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="J72" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K72" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L72" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="M72" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="N72" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="O72" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="P72" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
@@ -6535,69 +6655,161 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
+        <v>188</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2680</v>
+      </c>
+      <c r="D73" s="1">
+        <v>100</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H73" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="I73" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="K73" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L73" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="M73" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="N73" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="O73" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="P73" s="25" t="s">
+        <v>202</v>
+      </c>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1771</v>
+      </c>
+      <c r="D74" s="1">
+        <v>100</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H74" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I74" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J74" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K74" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="L74" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="M74" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="N74" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="O74" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="P74" s="17" t="s">
+        <v>196</v>
+      </c>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D75" s="1">
+        <v>100</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I75" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K75" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="L75" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="M75" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="N75" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="O75" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="P75" s="27" t="s">
+        <v>224</v>
+      </c>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
@@ -6625,6 +6837,98 @@
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
     </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L37:M37"/>

</xml_diff>